<commit_message>
Adding json formating to list of varianles and reference to source datasets
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="160">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">Datasets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Number of confirmed cases for the respective pathogen and reporting period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset 1, Dataset 2, Dataset 3</t>
   </si>
   <si>
     <t xml:space="preserve">Observation</t>
@@ -864,18 +870,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +899,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -900,1630 +908,1933 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>55</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G87" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="B88" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="B92" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G92" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="B93" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new methos for reseting json variable list
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">01. Cases</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of Cases</t>
+    <t xml:space="preserve">Number of Cases</t>
   </si>
   <si>
     <t xml:space="preserve">Number of confirmed cases for the respective pathogen and reporting period</t>
@@ -67,219 +67,7 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"N° of Cases", "modifiers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:[{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">variable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Case Status", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">value</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Confirmed"}]}, {"alias":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Cases at onset of symptomps date", "variable":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">N° of Cases", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">modifiers":[{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"variable":</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"period type", </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"value"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:"Onset of symptomps date"}]}]</t>
-    </r>
+    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -311,32 +99,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[{"15 days Incidence rate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
-    </r>
+    <t xml:space="preserve">[{"15 days Incidence rate":{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
   </si>
   <si>
     <t xml:space="preserve">Rt number</t>
@@ -348,7 +111,7 @@
     <t xml:space="preserve">[]</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of PPE Protective equipment</t>
+    <t xml:space="preserve">Number of PPE Protective equipment</t>
   </si>
   <si>
     <t xml:space="preserve">Resources</t>
@@ -375,7 +138,7 @@
     <t xml:space="preserve">02. Deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of deaths</t>
+    <t xml:space="preserve">Number of deaths</t>
   </si>
   <si>
     <t xml:space="preserve">Dead status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, Pathogen, Care facility, Eeference population, Period, Period type</t>
@@ -390,7 +153,7 @@
     <t xml:space="preserve">03. Patients</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of infected patients</t>
+    <t xml:space="preserve">Number of infected patients</t>
   </si>
   <si>
     <t xml:space="preserve">Care facility, Care facility type, Bed type, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Patient Status, Treatment received,  Vaccination status, External id, Pathogen, Period, Period type</t>
@@ -399,7 +162,7 @@
     <t xml:space="preserve">03. Patient</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of non-infected patients </t>
+    <t xml:space="preserve">Number of non-infected patients </t>
   </si>
   <si>
     <t xml:space="preserve">Care facility, Bed type, Vaccination status, External id, Reporting period, Pathogen, Period, Period type</t>
@@ -414,7 +177,7 @@
     <t xml:space="preserve">Care facility, External id, Pathogen, Period, Period type</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of hospital staff</t>
+    <t xml:space="preserve">Number of hospital staff</t>
   </si>
   <si>
     <t xml:space="preserve">Stafff type, Staff subtype, Care facility, Pathogen vaccination status, Pathogen, Period</t>
@@ -429,7 +192,7 @@
     <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Care facility, Period</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of hospital resources dependencies</t>
+    <t xml:space="preserve">Number of hospital resources dependencies</t>
   </si>
   <si>
     <t xml:space="preserve">Base resource, reference resource, Care facility, Period</t>
@@ -462,7 +225,7 @@
     <t xml:space="preserve">Positivity rate</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of test staff</t>
+    <t xml:space="preserve">Number of test staff</t>
   </si>
   <si>
     <t xml:space="preserve">Stafff type, Staff subtype, Test facility, Pathogen, Vaccination status, Pathogen, Period</t>
@@ -474,7 +237,7 @@
     <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Test facility, Period</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of test resources dependencies</t>
+    <t xml:space="preserve">Number of test resources dependencies</t>
   </si>
   <si>
     <t xml:space="preserve">Base resource, reference resource, Test facility, Period</t>
@@ -522,13 +285,13 @@
     <t xml:space="preserve">06. Contact tracing</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of index cases studied </t>
+    <t xml:space="preserve">Number of index cases studied </t>
   </si>
   <si>
     <t xml:space="preserve">Nº of contacts, secondary and terciary cases per index case</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of clusters found (and cluster type - definition)</t>
+    <t xml:space="preserve">Number of clusters found (and cluster type - definition)</t>
   </si>
   <si>
     <t xml:space="preserve">Confirmed cases that had travel during infectious period</t>
@@ -591,7 +354,7 @@
     <t xml:space="preserve">Severity of victims (at call and scene)</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of calls from people declared as confirm case</t>
+    <t xml:space="preserve">Number of calls from people declared as confirm case</t>
   </si>
   <si>
     <t xml:space="preserve">Monitoring of symptoms from emergency calls</t>
@@ -645,7 +408,7 @@
     <t xml:space="preserve">11. Measures</t>
   </si>
   <si>
-    <t xml:space="preserve">N° of people entering to the country (by origin)</t>
+    <t xml:space="preserve">Number of people entering to the country (by origin)</t>
   </si>
   <si>
     <t xml:space="preserve">Mitigation measures and policies</t>
@@ -764,7 +527,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -785,11 +548,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -872,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
1. implementing list of variables as dico 2. initializing standardizer
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$102</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="161">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -68,6 +71,15 @@
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[]</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -108,9 +120,6 @@
     <t xml:space="preserve">Calculation Period, Variant, Location, Pathogen, Period, Period type</t>
   </si>
   <si>
-    <t xml:space="preserve">[]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of PPE Protective equipment</t>
   </si>
   <si>
@@ -259,9 +268,6 @@
   </si>
   <si>
     <t xml:space="preserve">Doses injected by age group, risk group, and brand/type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characteristic</t>
   </si>
   <si>
     <t xml:space="preserve">Doses by vendor, batch</t>
@@ -623,25 +629,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="39.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -704,20 +716,12 @@
         <v>16</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,17 +729,17 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -756,16 +760,16 @@
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,55 +777,55 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
@@ -831,18 +835,18 @@
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
@@ -852,48 +856,48 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -906,15 +910,15 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>43</v>
@@ -927,42 +931,42 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>48</v>
@@ -972,45 +976,45 @@
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>53</v>
@@ -1020,45 +1024,45 @@
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>59</v>
@@ -1071,18 +1075,18 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>60</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>61</v>
@@ -1092,42 +1096,42 @@
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>64</v>
@@ -1137,21 +1141,21 @@
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>66</v>
@@ -1161,42 +1165,48 @@
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
@@ -1206,15 +1216,15 @@
         <v>12</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -1224,15 +1234,15 @@
         <v>12</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1242,30 +1252,30 @@
         <v>12</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>75</v>
@@ -1275,15 +1285,15 @@
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>76</v>
@@ -1293,15 +1303,15 @@
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>77</v>
@@ -1311,15 +1321,15 @@
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>78</v>
@@ -1329,15 +1339,15 @@
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>79</v>
@@ -1350,12 +1360,12 @@
         <v>17</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>80</v>
@@ -1365,33 +1375,33 @@
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>83</v>
@@ -1401,15 +1411,15 @@
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>84</v>
@@ -1419,15 +1429,15 @@
         <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>85</v>
@@ -1437,15 +1447,15 @@
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>86</v>
@@ -1455,15 +1465,15 @@
         <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>87</v>
@@ -1473,15 +1483,15 @@
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>88</v>
@@ -1491,15 +1501,15 @@
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>89</v>
@@ -1512,12 +1522,12 @@
         <v>17</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>90</v>
@@ -1527,33 +1537,33 @@
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>93</v>
@@ -1566,12 +1576,12 @@
         <v>12</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>94</v>
@@ -1581,15 +1591,15 @@
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>95</v>
@@ -1599,15 +1609,15 @@
         <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>96</v>
@@ -1617,15 +1627,15 @@
         <v>11</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>97</v>
@@ -1635,15 +1645,15 @@
         <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>98</v>
@@ -1653,15 +1663,15 @@
         <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>99</v>
@@ -1671,33 +1681,33 @@
         <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>103</v>
@@ -1710,12 +1720,12 @@
         <v>12</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>104</v>
@@ -1725,15 +1735,15 @@
         <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>105</v>
@@ -1743,15 +1753,15 @@
         <v>11</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>106</v>
@@ -1761,33 +1771,33 @@
         <v>11</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>109</v>
@@ -1800,12 +1810,12 @@
         <v>12</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>110</v>
@@ -1815,15 +1825,15 @@
         <v>11</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>111</v>
@@ -1833,15 +1843,15 @@
         <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>112</v>
@@ -1851,33 +1861,33 @@
         <v>11</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>115</v>
@@ -1890,12 +1900,12 @@
         <v>12</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>116</v>
@@ -1908,12 +1918,12 @@
         <v>12</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>117</v>
@@ -1923,15 +1933,15 @@
         <v>11</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>118</v>
@@ -1941,15 +1951,15 @@
         <v>11</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>119</v>
@@ -1959,15 +1969,15 @@
         <v>11</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>120</v>
@@ -1977,15 +1987,15 @@
         <v>11</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>121</v>
@@ -1995,33 +2005,33 @@
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>124</v>
@@ -2034,12 +2044,12 @@
         <v>12</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>125</v>
@@ -2049,15 +2059,15 @@
         <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>126</v>
@@ -2067,33 +2077,33 @@
         <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>129</v>
@@ -2106,12 +2116,12 @@
         <v>12</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>130</v>
@@ -2121,15 +2131,15 @@
         <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>131</v>
@@ -2139,15 +2149,15 @@
         <v>11</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>132</v>
@@ -2157,15 +2167,15 @@
         <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>133</v>
@@ -2175,15 +2185,15 @@
         <v>11</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>134</v>
@@ -2193,15 +2203,15 @@
         <v>11</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>135</v>
@@ -2211,15 +2221,15 @@
         <v>11</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>136</v>
@@ -2229,15 +2239,15 @@
         <v>11</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>137</v>
@@ -2247,15 +2257,15 @@
         <v>11</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>138</v>
@@ -2265,51 +2275,51 @@
         <v>11</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>143</v>
@@ -2319,15 +2329,15 @@
         <v>11</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>144</v>
@@ -2337,15 +2347,15 @@
         <v>11</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>145</v>
@@ -2355,15 +2365,15 @@
         <v>11</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>146</v>
@@ -2373,15 +2383,15 @@
         <v>11</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>147</v>
@@ -2391,15 +2401,15 @@
         <v>11</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>148</v>
@@ -2409,15 +2419,15 @@
         <v>11</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>149</v>
@@ -2427,15 +2437,15 @@
         <v>11</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>150</v>
@@ -2445,15 +2455,15 @@
         <v>11</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>151</v>
@@ -2463,15 +2473,15 @@
         <v>11</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>152</v>
@@ -2481,33 +2491,33 @@
         <v>11</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>155</v>
@@ -2517,15 +2527,15 @@
         <v>11</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>156</v>
@@ -2535,15 +2545,15 @@
         <v>11</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>157</v>
@@ -2553,15 +2563,15 @@
         <v>11</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>158</v>
@@ -2571,15 +2581,15 @@
         <v>11</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>159</v>
@@ -2589,19 +2599,39 @@
         <v>11</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H102"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the df2var method in DataframeReader actor
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charline CLAIN\Documents\PANDEM\pandem-source\pandem2source\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2702056-9BA1-4D7B-A106-CD0C4B78073B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,63 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="160">
-  <si>
-    <t xml:space="preserve">Data Family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datasets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linked Attributes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aliases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01. Cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of confirmed cases for the respective pathogen and reporting period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dataset 1, Dataset 2, Dataset 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">people</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidence rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">people/people</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="164">
+  <si>
+    <t>Data Family</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Datasets</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Linked Attributes</t>
+  </si>
+  <si>
+    <t>Aliases</t>
+  </si>
+  <si>
+    <t>01. Cases</t>
+  </si>
+  <si>
+    <t>Number of Cases</t>
+  </si>
+  <si>
+    <t>Number of confirmed cases for the respective pathogen and reporting period</t>
+  </si>
+  <si>
+    <t>Dataset 1, Dataset 2, Dataset 3</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
+  </si>
+  <si>
+    <t>[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
+  </si>
+  <si>
+    <t>Incidence rate</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>people/people</t>
   </si>
   <si>
     <r>
@@ -95,459 +100,453 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Period, Period type</t>
+      <t>Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Period, Period type</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">[{"15 days Incidence rate":{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rt number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculation Period, Variant, Location, Pathogen, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of PPE Protective equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units/time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location, Resource type, Unit, Pathogen, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needs of PPE Protective equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outbreak Id (if associated to known outbreak)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location, Pathogen, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02. Deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of deaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dead status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, Pathogen, Care facility, Eeference population, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mortality rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculation period, Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Care facility, External id, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03. Patients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of infected patients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Care facility, Care facility type, Bed type, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Patient Status, Treatment received,  Vaccination status, External id, Pathogen, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03. Patient</t>
+    <t>[{"15 days Incidence rate":{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
+  </si>
+  <si>
+    <t>Rt number</t>
+  </si>
+  <si>
+    <t>Calculation Period, Variant, Location, Pathogen, Period, Period type</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Number of PPE Protective equipment</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Units/time</t>
+  </si>
+  <si>
+    <t>Location, Resource type, Unit, Pathogen, Period</t>
+  </si>
+  <si>
+    <t>Needs of PPE Protective equipment</t>
+  </si>
+  <si>
+    <t>Outbreak Id (if associated to known outbreak)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Location, Pathogen, Period, Period type</t>
+  </si>
+  <si>
+    <t>02. Deaths</t>
+  </si>
+  <si>
+    <t>Number of deaths</t>
+  </si>
+  <si>
+    <t>Dead status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, Pathogen, Care facility, Eeference population, Period, Period type</t>
+  </si>
+  <si>
+    <t>Mortality rates</t>
+  </si>
+  <si>
+    <t>Calculation period, Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Care facility, External id, Period, Period type</t>
+  </si>
+  <si>
+    <t>03. Patients</t>
+  </si>
+  <si>
+    <t>Number of infected patients</t>
+  </si>
+  <si>
+    <t>Care facility, Care facility type, Bed type, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Patient Status, Treatment received,  Vaccination status, External id, Pathogen, Period, Period type</t>
+  </si>
+  <si>
+    <t>03. Patient</t>
   </si>
   <si>
     <t xml:space="preserve">Number of non-infected patients </t>
   </si>
   <si>
-    <t xml:space="preserve">Care facility, Bed type, Vaccination status, External id, Reporting period, Pathogen, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Length of stay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Care facility, External id, Pathogen, Period, Period type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of hospital staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stafff type, Staff subtype, Care facility, Pathogen vaccination status, Pathogen, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qty of hospital resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Care facility, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of hospital resources dependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base resource, reference resource, Care facility, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beds occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource type, resource subtype,  Care facility, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04.Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of tests performed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidemiological surveys Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epidemiological survey question, External Id, Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Positivity rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of test staff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stafff type, Staff subtype, Test facility, Pathogen, Vaccination status, Pathogen, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qty of test resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Test facility, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of test resources dependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base resource, reference resource, Test facility, Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05. Vaccination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses injected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">people that has received at least one dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People fully vaccinated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses scheduled and target population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses injected by age group, risk group, and brand/type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characteristic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses by vendor, batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses injected by occupation (HCW an other essential professionals...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doses injected in high risk individuals - potential risk factors (immunosuppressed, comorbidities, pregnant women, elderly...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccination Side effects AEFI observed and severity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccination progress (proportion of vaccinated, overall, by age and risk group)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccination resources (Staff, centres, supplies)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06. Contact tracing</t>
+    <t>Care facility, Bed type, Vaccination status, External id, Reporting period, Pathogen, Period, Period type</t>
+  </si>
+  <si>
+    <t>Length of stay</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Care facility, External id, Pathogen, Period, Period type</t>
+  </si>
+  <si>
+    <t>Number of hospital staff</t>
+  </si>
+  <si>
+    <t>Stafff type, Staff subtype, Care facility, Pathogen vaccination status, Pathogen, Period</t>
+  </si>
+  <si>
+    <t>Qty of hospital resources</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Resource type, resource subtype, Depletion mode, Care facility, Period</t>
+  </si>
+  <si>
+    <t>Number of hospital resources dependencies</t>
+  </si>
+  <si>
+    <t>Base resource, reference resource, Care facility, Period</t>
+  </si>
+  <si>
+    <t>Beds occupancy</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Resource type, resource subtype,  Care facility, Period</t>
+  </si>
+  <si>
+    <t>04.Tests</t>
+  </si>
+  <si>
+    <t>Number of tests performed</t>
+  </si>
+  <si>
+    <t>Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
+  </si>
+  <si>
+    <t>Epidemiological surveys Answer</t>
+  </si>
+  <si>
+    <t>Epidemiological survey question, External Id, Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
+  </si>
+  <si>
+    <t>Positivity rate</t>
+  </si>
+  <si>
+    <t>Number of test staff</t>
+  </si>
+  <si>
+    <t>Stafff type, Staff subtype, Test facility, Pathogen, Vaccination status, Pathogen, Period</t>
+  </si>
+  <si>
+    <t>Qty of test resources</t>
+  </si>
+  <si>
+    <t>Resource type, resource subtype, Depletion mode, Test facility, Period</t>
+  </si>
+  <si>
+    <t>Number of test resources dependencies</t>
+  </si>
+  <si>
+    <t>Base resource, reference resource, Test facility, Period</t>
+  </si>
+  <si>
+    <t>05. Vaccination</t>
+  </si>
+  <si>
+    <t>Doses injected</t>
+  </si>
+  <si>
+    <t>people that has received at least one dose</t>
+  </si>
+  <si>
+    <t>People fully vaccinated</t>
+  </si>
+  <si>
+    <t>Doses scheduled and target population</t>
+  </si>
+  <si>
+    <t>Doses injected by age group, risk group, and brand/type</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>Doses by vendor, batch</t>
+  </si>
+  <si>
+    <t>Doses injected by occupation (HCW an other essential professionals...)</t>
+  </si>
+  <si>
+    <t>Doses injected in high risk individuals - potential risk factors (immunosuppressed, comorbidities, pregnant women, elderly...)</t>
+  </si>
+  <si>
+    <t>Vaccination Side effects AEFI observed and severity</t>
+  </si>
+  <si>
+    <t>Vaccination progress (proportion of vaccinated, overall, by age and risk group)</t>
+  </si>
+  <si>
+    <t>Vaccination resources (Staff, centres, supplies)</t>
+  </si>
+  <si>
+    <t>06. Contact tracing</t>
   </si>
   <si>
     <t xml:space="preserve">Number of index cases studied </t>
   </si>
   <si>
-    <t xml:space="preserve">Nº of contacts, secondary and terciary cases per index case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of clusters found (and cluster type - definition)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirmed cases that had travel during infectious period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Types of contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact tracing details at individual level: travel, contacts, date of isolation, date of quarantine, transmission chains...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluster identification and characterisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notification delay (onset of symptoms - notification date)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact tracers (staff working in contact tracing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07. Lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of test performed (overall and by individual)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed of spread of variants (proportion among overall cases)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seroprevalence (and test type)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seaway water virus presence (and levels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mutations/Sequences spread and distributions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibility to link lab data with cases/patient data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possibility to associate lab data with aggregated epidemiological data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensibility &amp; specificity of test methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08. Emergency calls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitoring number of emergency calls (overall and by syndrome)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparison current situation with peacetime symptoms, notifications and diagnostic rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Severity of victims (at call and scene)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of calls from people declared as confirm case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monitoring of symptoms from emergency calls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09. First response</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoing emergencies (types)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visits to GP with compatible symptoms (disease X)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Details/type of protocol applied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public health Staff (surveillance, prevention and control activities..)</t>
+    <t>Nº of contacts, secondary and terciary cases per index case</t>
+  </si>
+  <si>
+    <t>Number of clusters found (and cluster type - definition)</t>
+  </si>
+  <si>
+    <t>Confirmed cases that had travel during infectious period</t>
+  </si>
+  <si>
+    <t>Types of contact</t>
+  </si>
+  <si>
+    <t>Contact tracing details at individual level: travel, contacts, date of isolation, date of quarantine, transmission chains...</t>
+  </si>
+  <si>
+    <t>Cluster identification and characterisation</t>
+  </si>
+  <si>
+    <t>Notification delay (onset of symptoms - notification date)</t>
+  </si>
+  <si>
+    <t>Contact tracers (staff working in contact tracing)</t>
+  </si>
+  <si>
+    <t>07. Lab</t>
+  </si>
+  <si>
+    <t>Number of test performed (overall and by individual)</t>
+  </si>
+  <si>
+    <t>Speed of spread of variants (proportion among overall cases)</t>
+  </si>
+  <si>
+    <t>seroprevalence (and test type)</t>
+  </si>
+  <si>
+    <t>Seaway water virus presence (and levels)</t>
+  </si>
+  <si>
+    <t>Mutations/Sequences spread and distributions</t>
+  </si>
+  <si>
+    <t>Possibility to link lab data with cases/patient data</t>
+  </si>
+  <si>
+    <t>Possibility to associate lab data with aggregated epidemiological data</t>
+  </si>
+  <si>
+    <t>Sensibility &amp; specificity of test methods</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>08. Emergency calls</t>
+  </si>
+  <si>
+    <t>Monitoring number of emergency calls (overall and by syndrome)</t>
+  </si>
+  <si>
+    <t>Comparison current situation with peacetime symptoms, notifications and diagnostic rates</t>
+  </si>
+  <si>
+    <t>Severity of victims (at call and scene)</t>
+  </si>
+  <si>
+    <t>Number of calls from people declared as confirm case</t>
+  </si>
+  <si>
+    <t>Monitoring of symptoms from emergency calls</t>
+  </si>
+  <si>
+    <t>09. First response</t>
+  </si>
+  <si>
+    <t>Ongoing emergencies (types)</t>
+  </si>
+  <si>
+    <t>Visits to GP with compatible symptoms (disease X)</t>
+  </si>
+  <si>
+    <t>Details/type of protocol applied</t>
+  </si>
+  <si>
+    <t>Public health Staff (surveillance, prevention and control activities..)</t>
   </si>
   <si>
     <t xml:space="preserve">Emergency Staff </t>
   </si>
   <si>
-    <t xml:space="preserve">10. Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient transportation type (for suspicious or confirmed cases)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current ambulance activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient transfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport statistics (duration, times)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport resources (ambulances)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ambulances / type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass patient transport threshold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass patient transport protocols</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11. Measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of people entering to the country (by origin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mitigation measures and policies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measure details: type (e.g. lockdown), start - end, place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Border rules/laws</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12. Population study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adherence to prevention and control measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is people understanding public health communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alerts &amp; Early warning signals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social media custom analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccination acceptance willingness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">level of trust in the Government and institutions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measure social impact (psychological, lifestyle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indirect impact on health (other notifiable disease, disruption of services, indirect deaths and morbidity...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People beliefs and opinions on pandemic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consulted public information sites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People information needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13. Referentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denominators for potential risk factors or individuals at risk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pathogen specific referential epidemiological parameters
+    <t>10. Transport</t>
+  </si>
+  <si>
+    <t>Patient transportation type (for suspicious or confirmed cases)</t>
+  </si>
+  <si>
+    <t>Current ambulance activity</t>
+  </si>
+  <si>
+    <t>Patient transfers</t>
+  </si>
+  <si>
+    <t>Transport statistics (duration, times)</t>
+  </si>
+  <si>
+    <t>Transport resources (ambulances)</t>
+  </si>
+  <si>
+    <t>Ambulances / type</t>
+  </si>
+  <si>
+    <t>Mass patient transport threshold</t>
+  </si>
+  <si>
+    <t>Mass patient transport protocols</t>
+  </si>
+  <si>
+    <t>11. Measures</t>
+  </si>
+  <si>
+    <t>Number of people entering to the country (by origin)</t>
+  </si>
+  <si>
+    <t>Mitigation measures and policies</t>
+  </si>
+  <si>
+    <t>Measure details: type (e.g. lockdown), start - end, place</t>
+  </si>
+  <si>
+    <t>Border rules/laws</t>
+  </si>
+  <si>
+    <t>12. Population study</t>
+  </si>
+  <si>
+    <t>Adherence to prevention and control measures</t>
+  </si>
+  <si>
+    <t>Is people understanding public health communication</t>
+  </si>
+  <si>
+    <t>Alerts &amp; Early warning signals</t>
+  </si>
+  <si>
+    <t>Social media custom analysis</t>
+  </si>
+  <si>
+    <t>Vaccination acceptance willingness</t>
+  </si>
+  <si>
+    <t>level of trust in the Government and institutions</t>
+  </si>
+  <si>
+    <t>Measure social impact (psychological, lifestyle)</t>
+  </si>
+  <si>
+    <t>indirect impact on health (other notifiable disease, disruption of services, indirect deaths and morbidity...)</t>
+  </si>
+  <si>
+    <t>People beliefs and opinions on pandemic</t>
+  </si>
+  <si>
+    <t>Most consulted public information sites</t>
+  </si>
+  <si>
+    <t>People information needs</t>
+  </si>
+  <si>
+    <t>13. Referentials</t>
+  </si>
+  <si>
+    <t>Denominators for potential risk factors or individuals at risk</t>
+  </si>
+  <si>
+    <t>Referential</t>
+  </si>
+  <si>
+    <t>pathogen specific referential epidemiological parameters
 (Host, vector, latency, contagiousness, Serial interval, Susceptibility...)</t>
   </si>
   <si>
-    <t xml:space="preserve">Symptoms &amp; signs by pathogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Care procedures (for new diseases)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variants (VOI, VOC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">denominators and maps for different Geographic location (local to international)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population denominators (age, sex, country of birth ... )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social determinants by area or case (country of birth, wealth, studies, occupation...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Care providers by area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shared guidelines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Places of infection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supplies for potential or confirmed efective medication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14. Metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable definitions (calcuation method, description)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data providers for dashboards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dashboard profile e.g. emergency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDPR compliance</t>
+    <t>Symptoms &amp; signs by pathogen</t>
+  </si>
+  <si>
+    <t>Care procedures (for new diseases)</t>
+  </si>
+  <si>
+    <t>Variants (VOI, VOC)</t>
+  </si>
+  <si>
+    <t>denominators and maps for different Geographic location (local to international)</t>
+  </si>
+  <si>
+    <t>Population denominators (age, sex, country of birth ... )</t>
+  </si>
+  <si>
+    <t>Social determinants by area or case (country of birth, wealth, studies, occupation...)</t>
+  </si>
+  <si>
+    <t>Care providers by area</t>
+  </si>
+  <si>
+    <t>User shared guidelines</t>
+  </si>
+  <si>
+    <t>Places of infection</t>
+  </si>
+  <si>
+    <t>supplies for potential or confirmed efective medication</t>
+  </si>
+  <si>
+    <t>14. Metadata</t>
+  </si>
+  <si>
+    <t>Variable definitions (calcuation method, description)</t>
+  </si>
+  <si>
+    <t>Source contact</t>
+  </si>
+  <si>
+    <t>Data owner</t>
+  </si>
+  <si>
+    <t>Data providers for dashboards</t>
+  </si>
+  <si>
+    <t>Dashboard profile e.g. emergency</t>
+  </si>
+  <si>
+    <t>GDPR compliance</t>
+  </si>
+  <si>
+    <t>Reporting date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>iso country code</t>
+  </si>
+  <si>
+    <t>Location code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -565,7 +564,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -573,78 +572,346 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.52"/>
+    <col min="1" max="1" width="17.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" style="1" customWidth="1"/>
+    <col min="6" max="1024" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,7 +937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -696,180 +963,161 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -879,21 +1127,21 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -906,114 +1154,114 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
@@ -1023,216 +1271,234 @@
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1245,66 +1511,66 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
@@ -1317,12 +1583,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -1335,66 +1601,66 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
@@ -1407,30 +1673,30 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
@@ -1443,156 +1709,156 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
@@ -1605,138 +1871,138 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
@@ -1749,48 +2015,48 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
@@ -1803,12 +2069,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
@@ -1821,264 +2087,264 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -2091,84 +2357,84 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
@@ -2181,12 +2447,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
@@ -2199,12 +2465,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
@@ -2217,12 +2483,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
@@ -2235,102 +2501,102 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:8" ht="66" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
@@ -2343,12 +2609,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
@@ -2361,12 +2627,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
@@ -2379,12 +2645,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
@@ -2397,12 +2663,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
@@ -2415,12 +2681,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
@@ -2433,120 +2699,120 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
@@ -2559,12 +2825,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
@@ -2577,12 +2843,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
@@ -2595,11 +2861,64 @@
         <v>23</v>
       </c>
     </row>
+    <row r="102" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
modification de la list-of-variables excel
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$102</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$105</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="165">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -73,13 +73,28 @@
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
   </si>
   <si>
+    <t xml:space="preserve">Pathogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referential alias </t>
+  </si>
+  <si>
     <t xml:space="preserve">Case status</t>
   </si>
   <si>
     <t xml:space="preserve">Characteristic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[]</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -466,9 +481,6 @@
   </si>
   <si>
     <t xml:space="preserve">Denominators for potential risk factors or individuals at risk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referential</t>
   </si>
   <si>
     <t xml:space="preserve">pathogen specific referential epidemiological parameters
@@ -638,16 +650,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
@@ -724,7 +736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -732,65 +744,44 @@
         <v>19</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
@@ -801,44 +792,44 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
@@ -846,23 +837,23 @@
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>18</v>
@@ -870,34 +861,34 @@
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -907,10 +898,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>18</v>
@@ -918,10 +909,10 @@
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -934,7 +925,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>18</v>
@@ -942,23 +933,23 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>18</v>
@@ -966,23 +957,23 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>18</v>
@@ -990,23 +981,23 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>18</v>
@@ -1014,23 +1005,23 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>18</v>
@@ -1038,23 +1029,23 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>18</v>
@@ -1062,23 +1053,23 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>18</v>
@@ -1086,23 +1077,23 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>18</v>
@@ -1110,20 +1101,23 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>18</v>
@@ -1131,7 +1125,7 @@
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>64</v>
@@ -1141,10 +1135,10 @@
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>65</v>
@@ -1155,7 +1149,7 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>66</v>
@@ -1165,10 +1159,10 @@
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>67</v>
@@ -1179,7 +1173,7 @@
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>68</v>
@@ -1189,13 +1183,10 @@
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>18</v>
@@ -1203,17 +1194,23 @@
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>18</v>
@@ -1221,17 +1218,23 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>18</v>
@@ -1239,7 +1242,7 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>73</v>
@@ -1249,7 +1252,13 @@
         <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>18</v>
@@ -1257,10 +1266,10 @@
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
@@ -1273,19 +1282,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>18</v>
@@ -1293,71 +1302,71 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>18</v>
@@ -1365,71 +1374,71 @@
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>18</v>
@@ -1437,28 +1446,28 @@
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
@@ -1471,109 +1480,109 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>18</v>
@@ -1581,46 +1590,46 @@
     </row>
     <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
@@ -1633,55 +1642,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>18</v>
@@ -1689,17 +1698,17 @@
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>18</v>
@@ -1707,7 +1716,7 @@
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>103</v>
@@ -1717,15 +1726,15 @@
         <v>11</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>104</v>
@@ -1735,7 +1744,7 @@
         <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>18</v>
@@ -1743,7 +1752,7 @@
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>105</v>
@@ -1753,18 +1762,18 @@
         <v>11</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
@@ -1777,19 +1786,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>18</v>
@@ -1797,28 +1806,28 @@
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
@@ -1833,89 +1842,89 @@
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>18</v>
@@ -1923,35 +1932,35 @@
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>18</v>
@@ -1959,17 +1968,17 @@
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>18</v>
@@ -1977,17 +1986,17 @@
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>18</v>
@@ -1995,17 +2004,17 @@
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>18</v>
@@ -2013,17 +2022,17 @@
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>18</v>
@@ -2031,17 +2040,17 @@
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>18</v>
@@ -2049,35 +2058,35 @@
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>18</v>
@@ -2085,17 +2094,17 @@
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>18</v>
@@ -2106,7 +2115,7 @@
         <v>128</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
@@ -2124,14 +2133,14 @@
         <v>128</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>18</v>
@@ -2142,14 +2151,14 @@
         <v>128</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>18</v>
@@ -2157,53 +2166,53 @@
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>18</v>
@@ -2211,53 +2220,53 @@
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>18</v>
@@ -2265,61 +2274,61 @@
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>142</v>
+        <v>25</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>143</v>
@@ -2329,7 +2338,7 @@
         <v>11</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>18</v>
@@ -2337,7 +2346,7 @@
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>144</v>
@@ -2347,177 +2356,177 @@
         <v>11</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>155</v>
@@ -2527,7 +2536,7 @@
         <v>11</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>18</v>
@@ -2535,7 +2544,7 @@
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>156</v>
@@ -2545,15 +2554,15 @@
         <v>11</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>157</v>
@@ -2563,25 +2572,25 @@
         <v>11</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>18</v>
@@ -2589,17 +2598,17 @@
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>18</v>
@@ -2607,24 +2616,78 @@
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H102"/>
+  <autoFilter ref="A1:H105"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1- Modification du fichier des varaibles excel 2- Modification du country_name avec country_code 3- changement du separateur pour le nom des variables
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$105</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$107</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="168">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -82,13 +82,22 @@
     <t xml:space="preserve">[]</t>
   </si>
   <si>
+    <t xml:space="preserve">Geo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country code</t>
   </si>
   <si>
+    <t xml:space="preserve">Line number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country name</t>
   </si>
   <si>
-    <t xml:space="preserve">Referential alias </t>
+    <t xml:space="preserve">Referential alias</t>
   </si>
   <si>
     <t xml:space="preserve">Case status</t>
@@ -650,10 +659,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -762,10 +771,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -776,60 +782,47 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
@@ -840,23 +833,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,44 +857,44 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>18</v>
@@ -909,47 +902,47 @@
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>18</v>
@@ -957,10 +950,10 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -973,7 +966,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>18</v>
@@ -981,23 +974,23 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>18</v>
@@ -1008,7 +1001,7 @@
         <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
@@ -1018,10 +1011,10 @@
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>18</v>
@@ -1029,23 +1022,23 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>18</v>
@@ -1053,23 +1046,23 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>18</v>
@@ -1077,23 +1070,23 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>18</v>
@@ -1101,23 +1094,23 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>18</v>
@@ -1125,23 +1118,23 @@
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>18</v>
@@ -1149,23 +1142,23 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>18</v>
@@ -1173,20 +1166,23 @@
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>18</v>
@@ -1194,7 +1190,7 @@
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>69</v>
@@ -1204,10 +1200,10 @@
         <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>70</v>
@@ -1218,7 +1214,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>71</v>
@@ -1228,13 +1224,10 @@
         <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>18</v>
@@ -1242,23 +1235,23 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>18</v>
@@ -1266,17 +1259,23 @@
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>18</v>
@@ -1284,17 +1283,23 @@
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>18</v>
@@ -1302,10 +1307,10 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
@@ -1320,10 +1325,10 @@
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
@@ -1336,19 +1341,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>18</v>
@@ -1356,115 +1361,115 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>88</v>
@@ -1474,15 +1479,15 @@
         <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>89</v>
@@ -1492,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>18</v>
@@ -1500,17 +1505,17 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>18</v>
@@ -1518,17 +1523,17 @@
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>18</v>
@@ -1536,28 +1541,28 @@
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
@@ -1572,53 +1577,53 @@
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>18</v>
@@ -1626,7 +1631,7 @@
     </row>
     <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>98</v>
@@ -1636,7 +1641,7 @@
         <v>11</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>18</v>
@@ -1644,7 +1649,7 @@
     </row>
     <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>99</v>
@@ -1654,36 +1659,36 @@
         <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
@@ -1698,71 +1703,71 @@
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>18</v>
@@ -1770,64 +1775,64 @@
     </row>
     <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
@@ -1842,17 +1847,17 @@
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>18</v>
@@ -1860,7 +1865,7 @@
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>114</v>
@@ -1876,9 +1881,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>115</v>
@@ -1888,7 +1893,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>18</v>
@@ -1896,17 +1901,17 @@
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>18</v>
@@ -1914,17 +1919,17 @@
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>18</v>
@@ -1932,17 +1937,17 @@
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>18</v>
@@ -1950,7 +1955,7 @@
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>120</v>
@@ -1960,7 +1965,7 @@
         <v>11</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>18</v>
@@ -1968,7 +1973,7 @@
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>121</v>
@@ -1978,18 +1983,18 @@
         <v>11</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
@@ -2004,17 +2009,17 @@
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>18</v>
@@ -2022,17 +2027,17 @@
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>18</v>
@@ -2040,17 +2045,17 @@
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>18</v>
@@ -2058,17 +2063,17 @@
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>18</v>
@@ -2076,17 +2081,17 @@
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>18</v>
@@ -2094,7 +2099,7 @@
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>129</v>
@@ -2104,7 +2109,7 @@
         <v>11</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>18</v>
@@ -2112,7 +2117,7 @@
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>130</v>
@@ -2122,25 +2127,25 @@
         <v>11</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>18</v>
@@ -2148,25 +2153,25 @@
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>134</v>
@@ -2176,15 +2181,15 @@
         <v>11</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>135</v>
@@ -2194,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>18</v>
@@ -2202,35 +2207,35 @@
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>18</v>
@@ -2238,35 +2243,35 @@
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>18</v>
@@ -2274,35 +2279,35 @@
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>18</v>
@@ -2310,35 +2315,35 @@
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>18</v>
@@ -2346,25 +2351,25 @@
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>146</v>
@@ -2374,15 +2379,15 @@
         <v>11</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>147</v>
@@ -2392,18 +2397,18 @@
         <v>11</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
@@ -2416,12 +2421,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
@@ -2436,10 +2441,10 @@
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
@@ -2452,12 +2457,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
@@ -2470,12 +2475,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
@@ -2490,10 +2495,10 @@
     </row>
     <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
@@ -2506,12 +2511,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
@@ -2524,19 +2529,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>18</v>
@@ -2544,43 +2549,43 @@
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>159</v>
@@ -2590,15 +2595,15 @@
         <v>11</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>160</v>
@@ -2608,18 +2613,18 @@
         <v>11</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
@@ -2634,10 +2639,10 @@
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
@@ -2652,10 +2657,10 @@
     </row>
     <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
@@ -2670,10 +2675,10 @@
     </row>
     <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
@@ -2686,8 +2691,44 @@
         <v>18</v>
       </c>
     </row>
+    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H105"/>
+  <autoFilter ref="A1:H107"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
running local_git acquisition and format reader csv
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$105</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$107</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="173">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Linked Attributes</t>
   </si>
   <si>
+    <t xml:space="preserve">Partrion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aliases</t>
   </si>
   <si>
@@ -70,6 +73,25 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">confi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">rmed_date, geo_code</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
   </si>
   <si>
@@ -82,19 +104,62 @@
     <t xml:space="preserve">[]</t>
   </si>
   <si>
+    <t xml:space="preserve">geo_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"alias":"Country Code", "variable":"Geo Code", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referential alias </t>
+  </si>
+  <si>
     <t xml:space="preserve">Country code</t>
   </si>
   <si>
-    <t xml:space="preserve">Country name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Referential alias </t>
+    <t xml:space="preserve">[{"alias":"Country Name", "variable":"Geo Name", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo_parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo_level</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Country, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">NUTS_1, NUTS_2, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NUTS_3</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Case status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characteristic</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -545,7 +610,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -566,6 +631,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -616,7 +686,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -627,6 +697,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -650,10 +724,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -693,290 +767,282 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,1716 +1050,1764 @@
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>18</v>
+        <v>67</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>18</v>
+        <v>70</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>18</v>
+        <v>64</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>18</v>
+        <v>75</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>18</v>
+        <v>78</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H103" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H105" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H105"/>
+  <autoFilter ref="A1:I107"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing dfreader to read covid19datahub data
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$107</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="174">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Linked Attributes</t>
   </si>
   <si>
-    <t xml:space="preserve">Partrion</t>
+    <t xml:space="preserve">Partition</t>
   </si>
   <si>
     <t xml:space="preserve">Aliases</t>
@@ -73,23 +73,7 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">confi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">rmed_date, geo_code</t>
-    </r>
+    <t xml:space="preserve">confirmed_date, geo_code</t>
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
@@ -104,13 +88,16 @@
     <t xml:space="preserve">[]</t>
   </si>
   <si>
-    <t xml:space="preserve">geo_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"alias":"Country Code", "variable":"Geo Code", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geo_name</t>
+    <t xml:space="preserve">13. Referentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geo Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"alias":"Iso Country Code 2", "variable":"Geo Code", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geo Name</t>
   </si>
   <si>
     <t xml:space="preserve">Referential alias </t>
@@ -122,44 +109,22 @@
     <t xml:space="preserve">[{"alias":"Country Name", "variable":"Geo Name", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
   </si>
   <si>
-    <t xml:space="preserve">geo_parent</t>
+    <t xml:space="preserve">Geo Parent</t>
   </si>
   <si>
     <t xml:space="preserve">Characteristic</t>
   </si>
   <si>
-    <t xml:space="preserve">geo_level</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Country, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">NUTS_1, NUTS_2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NUTS_3</t>
-    </r>
+    <t xml:space="preserve">Geo Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country, NUTS_1, NUTS_2, NUTS_3</t>
   </si>
   <si>
     <t xml:space="preserve">Case status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting Date</t>
   </si>
   <si>
     <t xml:space="preserve">Incidence rate</t>
@@ -540,9 +505,6 @@
   </si>
   <si>
     <t xml:space="preserve">People information needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13. Referentials</t>
   </si>
   <si>
     <t xml:space="preserve">Denominators for potential risk factors or individuals at risk</t>
@@ -699,8 +661,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -724,10 +686,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,69 +779,69 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
+      <c r="A4" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
+      <c r="A5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
+      <c r="A7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>20</v>
@@ -890,39 +852,31 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,23 +884,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,13 +915,13 @@
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>20</v>
@@ -978,20 +932,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>20</v>
@@ -1002,20 +956,20 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>20</v>
@@ -1023,10 +977,10 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1036,10 +990,10 @@
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>20</v>
@@ -1047,7 +1001,7 @@
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>50</v>
@@ -1057,10 +1011,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>51</v>
@@ -1071,23 +1025,23 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>20</v>
@@ -1095,10 +1049,10 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
@@ -1111,7 +1065,7 @@
         <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>20</v>
@@ -1119,7 +1073,7 @@
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>58</v>
@@ -1132,10 +1086,10 @@
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>20</v>
@@ -1143,20 +1097,20 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>62</v>
@@ -1167,7 +1121,7 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>63</v>
@@ -1177,13 +1131,13 @@
         <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>20</v>
@@ -1191,20 +1145,20 @@
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>67</v>
@@ -1215,7 +1169,7 @@
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>68</v>
@@ -1225,13 +1179,13 @@
         <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>20</v>
@@ -1239,23 +1193,23 @@
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>20</v>
@@ -1263,7 +1217,7 @@
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>74</v>
@@ -1276,7 +1230,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>75</v>
@@ -1287,7 +1241,7 @@
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>76</v>
@@ -1297,10 +1251,13 @@
         <v>12</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>20</v>
@@ -1308,23 +1265,20 @@
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>20</v>
@@ -1332,7 +1286,7 @@
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>79</v>
@@ -1342,10 +1296,10 @@
         <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>80</v>
@@ -1356,7 +1310,7 @@
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>81</v>
@@ -1366,10 +1320,10 @@
         <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>82</v>
@@ -1380,17 +1334,23 @@
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>20</v>
@@ -1398,10 +1358,10 @@
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
@@ -1416,10 +1376,10 @@
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
@@ -1434,10 +1394,10 @@
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -1452,17 +1412,17 @@
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>20</v>
@@ -1470,17 +1430,17 @@
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>20</v>
@@ -1488,53 +1448,53 @@
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>20</v>
@@ -1542,17 +1502,17 @@
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>20</v>
@@ -1560,17 +1520,17 @@
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>20</v>
@@ -1578,7 +1538,7 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>96</v>
@@ -1588,7 +1548,7 @@
         <v>12</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>20</v>
@@ -1596,17 +1556,17 @@
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>20</v>
@@ -1614,17 +1574,17 @@
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>20</v>
@@ -1632,17 +1592,17 @@
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>20</v>
@@ -1650,53 +1610,53 @@
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>20</v>
@@ -1704,17 +1664,17 @@
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>20</v>
@@ -1722,17 +1682,17 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>20</v>
@@ -1740,7 +1700,7 @@
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>106</v>
@@ -1750,7 +1710,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>20</v>
@@ -1758,10 +1718,10 @@
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
@@ -1776,17 +1736,17 @@
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>20</v>
@@ -1794,17 +1754,17 @@
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>20</v>
@@ -1812,17 +1772,17 @@
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>20</v>
@@ -1830,17 +1790,17 @@
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>20</v>
@@ -1848,17 +1808,17 @@
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>20</v>
@@ -1866,17 +1826,17 @@
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>20</v>
@@ -1884,17 +1844,17 @@
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>20</v>
@@ -1902,10 +1862,10 @@
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
@@ -1920,17 +1880,17 @@
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>20</v>
@@ -1938,17 +1898,17 @@
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>20</v>
@@ -1956,17 +1916,17 @@
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>20</v>
@@ -1974,7 +1934,7 @@
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>122</v>
@@ -1984,7 +1944,7 @@
         <v>12</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>20</v>
@@ -1992,10 +1952,10 @@
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
@@ -2010,17 +1970,17 @@
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>20</v>
@@ -2028,17 +1988,17 @@
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>20</v>
@@ -2046,17 +2006,17 @@
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>20</v>
@@ -2064,7 +2024,7 @@
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>128</v>
@@ -2074,7 +2034,7 @@
         <v>12</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>20</v>
@@ -2082,10 +2042,10 @@
     </row>
     <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
@@ -2100,10 +2060,10 @@
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
@@ -2118,17 +2078,17 @@
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>20</v>
@@ -2136,17 +2096,17 @@
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>20</v>
@@ -2154,17 +2114,17 @@
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>20</v>
@@ -2172,17 +2132,17 @@
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>20</v>
@@ -2190,17 +2150,17 @@
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>20</v>
@@ -2208,7 +2168,7 @@
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>137</v>
@@ -2218,7 +2178,7 @@
         <v>12</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>20</v>
@@ -2226,10 +2186,10 @@
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
@@ -2244,17 +2204,17 @@
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>20</v>
@@ -2262,17 +2222,17 @@
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>20</v>
@@ -2280,7 +2240,7 @@
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>142</v>
@@ -2290,7 +2250,7 @@
         <v>12</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>20</v>
@@ -2298,10 +2258,10 @@
     </row>
     <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
@@ -2316,17 +2276,17 @@
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>20</v>
@@ -2334,17 +2294,17 @@
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>20</v>
@@ -2352,17 +2312,17 @@
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>20</v>
@@ -2370,17 +2330,17 @@
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>20</v>
@@ -2388,53 +2348,53 @@
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>20</v>
@@ -2442,17 +2402,17 @@
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>20</v>
@@ -2460,17 +2420,17 @@
     </row>
     <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>20</v>
@@ -2478,7 +2438,7 @@
     </row>
     <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>154</v>
@@ -2488,15 +2448,15 @@
         <v>12</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>155</v>
@@ -2512,9 +2472,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>156</v>
@@ -2532,7 +2492,7 @@
     </row>
     <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>157</v>
@@ -2550,7 +2510,7 @@
     </row>
     <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>158</v>
@@ -2568,7 +2528,7 @@
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>159</v>
@@ -2586,7 +2546,7 @@
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>160</v>
@@ -2604,7 +2564,7 @@
     </row>
     <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>161</v>
@@ -2622,7 +2582,7 @@
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>162</v>
@@ -2640,7 +2600,7 @@
     </row>
     <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>163</v>
@@ -2650,7 +2610,7 @@
         <v>12</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>20</v>
@@ -2658,7 +2618,7 @@
     </row>
     <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>164</v>
@@ -2668,7 +2628,7 @@
         <v>12</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>20</v>
@@ -2676,7 +2636,7 @@
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>165</v>
@@ -2686,7 +2646,7 @@
         <v>12</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>20</v>
@@ -2694,17 +2654,17 @@
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>20</v>
@@ -2712,7 +2672,7 @@
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>168</v>
@@ -2730,7 +2690,7 @@
     </row>
     <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>169</v>
@@ -2748,7 +2708,7 @@
     </row>
     <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>170</v>
@@ -2766,7 +2726,7 @@
     </row>
     <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>171</v>
@@ -2784,7 +2744,7 @@
     </row>
     <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>172</v>
@@ -2800,8 +2760,26 @@
         <v>20</v>
       </c>
     </row>
+    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I107"/>
+  <autoFilter ref="A1:I108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fixing variable writer. first working sample with covid19-datahub
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
-    <t xml:space="preserve">confirmed_date, geo_code</t>
+    <t xml:space="preserve">reporting_date</t>
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
@@ -704,7 +704,7 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
1. including more variables from COVID19 datahub 2. Adding alias modifiers into storage
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$113</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$113</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="179">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Datasets</t>
-  </si>
-  <si>
     <t xml:space="preserve">Type</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t xml:space="preserve">Number of confirmed cases for the respective pathogen and reporting period</t>
   </si>
   <si>
-    <t xml:space="preserve">Dataset 1, Dataset 2, Dataset 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Observation</t>
   </si>
   <si>
@@ -73,10 +67,10 @@
     <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
   </si>
   <si>
-    <t xml:space="preserve">reporting_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
+    <t xml:space="preserve">reporting_date,case_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]},{"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Pathogen Code</t>
@@ -228,6 +222,37 @@
     <t xml:space="preserve">Care facility, Care facility type, Bed type, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Patient Status, Treatment received,  Vaccination status, External id, Pathogen, Period, Period type</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[{"alias":"number_of_icu_patients", "variable":"Number of infected_patients", "modifiers":[{"variable":"Severity", "value":"ICU"}]}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{"alias":"Number of patients with ventilator", "variable":"Number of infected patients", "modifiers":[{"variable":"Severity", "value":"With Ventilator"}]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Severity</t>
+  </si>
+  <si>
     <t xml:space="preserve">03. Patient</t>
   </si>
   <si>
@@ -318,10 +343,35 @@
     <t xml:space="preserve">Doses injected</t>
   </si>
   <si>
-    <t xml:space="preserve">people that has received at least one dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People fully vaccinated</t>
+    <t xml:space="preserve">People vaccinated</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[{"alias":"people that has received at least one dose", "variable":"People vaccinated", "modifiers":[{"variable":"Vaccination status", "value":"At least one dose"}]}, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{"alias":"People fully vaccinated", "variable":"People vaccinated", "modifiers":[{"variable":"Vaccination status", "value":"Fully vaccinated"}]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Doses scheduled and target population</t>
@@ -541,7 +591,7 @@
     <t xml:space="preserve">denominators and maps for different Geographic location (local to international)</t>
   </si>
   <si>
-    <t xml:space="preserve">Population denominators (age, sex, country of birth ... )</t>
+    <t xml:space="preserve">Population</t>
   </si>
   <si>
     <t xml:space="preserve">Social determinants by area or case (country of birth, wealth, studies, occupation...)</t>
@@ -701,10 +751,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -712,11 +762,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="39.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +781,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -744,777 +793,690 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>20</v>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>20</v>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>20</v>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>20</v>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>20</v>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="1" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>47</v>
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>90</v>
       </c>
@@ -1523,13 +1485,10 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,16 +1500,13 @@
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>90</v>
       </c>
@@ -1559,13 +1515,10 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,13 +1530,10 @@
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,13 +1545,10 @@
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,13 +1560,10 @@
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,13 +1575,10 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,16 +1590,13 @@
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>102</v>
       </c>
@@ -1667,13 +1605,10 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,13 +1620,10 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,13 +1635,10 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,16 +1650,13 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>102</v>
       </c>
@@ -1739,13 +1665,10 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,16 +1680,13 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
@@ -1775,13 +1695,10 @@
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,13 +1710,10 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,13 +1725,10 @@
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,13 +1740,10 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,16 +1755,13 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -1865,16 +1770,13 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
@@ -1883,16 +1785,13 @@
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
@@ -1901,13 +1800,10 @@
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,13 +1815,10 @@
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,16 +1830,13 @@
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>112</v>
       </c>
@@ -1955,13 +1845,10 @@
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I62" s="1" t="s">
-        <v>20</v>
+      <c r="H62" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,13 +1860,10 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,16 +1875,13 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
@@ -2009,13 +1890,10 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2027,16 +1905,13 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
         <v>122</v>
       </c>
@@ -2045,16 +1920,13 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>128</v>
       </c>
@@ -2063,13 +1935,10 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,16 +1950,13 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
         <v>128</v>
       </c>
@@ -2099,13 +1965,10 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,16 +1980,13 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>128</v>
       </c>
@@ -2135,13 +1995,10 @@
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,16 +2010,13 @@
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>134</v>
       </c>
@@ -2171,16 +2025,13 @@
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>134</v>
       </c>
@@ -2189,16 +2040,13 @@
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
         <v>134</v>
       </c>
@@ -2207,16 +2055,13 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>134</v>
       </c>
@@ -2225,16 +2070,13 @@
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>134</v>
       </c>
@@ -2243,16 +2085,13 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>134</v>
       </c>
@@ -2261,16 +2100,13 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>134</v>
       </c>
@@ -2279,13 +2115,10 @@
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I80" s="1" t="s">
-        <v>20</v>
+      <c r="H80" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,16 +2130,13 @@
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
         <v>143</v>
       </c>
@@ -2315,13 +2145,10 @@
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,16 +2160,13 @@
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
         <v>143</v>
       </c>
@@ -2351,16 +2175,13 @@
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I84" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H84" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
         <v>148</v>
       </c>
@@ -2369,13 +2190,10 @@
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2387,16 +2205,13 @@
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>148</v>
       </c>
@@ -2405,16 +2220,13 @@
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
         <v>148</v>
       </c>
@@ -2423,16 +2235,13 @@
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
         <v>148</v>
       </c>
@@ -2441,16 +2250,13 @@
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
         <v>148</v>
       </c>
@@ -2459,16 +2265,13 @@
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
         <v>148</v>
       </c>
@@ -2477,13 +2280,10 @@
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,16 +2295,13 @@
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
         <v>148</v>
       </c>
@@ -2513,16 +2310,13 @@
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
         <v>148</v>
       </c>
@@ -2531,16 +2325,13 @@
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
         <v>148</v>
       </c>
@@ -2549,229 +2340,193 @@
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E95" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I95" s="1" t="s">
-        <v>20</v>
+      <c r="H95" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>20</v>
+      <c r="H102" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>169</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I105" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H105" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I106" s="1" t="s">
-        <v>20</v>
+      <c r="H106" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E107" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>20</v>
+      <c r="H107" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,16 +2538,13 @@
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
         <v>172</v>
       </c>
@@ -2801,16 +2553,13 @@
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
         <v>172</v>
       </c>
@@ -2819,16 +2568,13 @@
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
         <v>172</v>
       </c>
@@ -2837,16 +2583,13 @@
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
         <v>172</v>
       </c>
@@ -2855,16 +2598,13 @@
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
         <v>172</v>
       </c>
@@ -2873,17 +2613,14 @@
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I113"/>
+  <autoFilter ref="A1:H113"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1. Fixing error preventing all attributes of measures to be displayed 2. Improving partitioning schema for some variables
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$113</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="164">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -64,10 +64,7 @@
     <t xml:space="preserve">people</t>
   </si>
   <si>
-    <t xml:space="preserve">Case status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, pathogen, vaccination status, Period, Period Type, Reference population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reporting_date,case_status</t>
+    <t xml:space="preserve">reporting_period,case_status</t>
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]},{"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
@@ -85,7 +82,7 @@
     <t xml:space="preserve">Pathogen Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Referential alias </t>
+    <t xml:space="preserve">Referential alias</t>
   </si>
   <si>
     <t xml:space="preserve">13. Referentials</t>
@@ -133,16 +130,7 @@
     <t xml:space="preserve">Case status</t>
   </si>
   <si>
-    <t xml:space="preserve">Reporting Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidence rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">people/people</t>
+    <t xml:space="preserve">Reporting Period</t>
   </si>
   <si>
     <r>
@@ -152,28 +140,45 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Calculation period, </t>
+      <t xml:space="preserve">[{"alias":"Reporting Date", "variable":"Reporting period", "modifiers":[{"variable":"Period Type", "value":"Date"}]}, </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{"alias":"Reporting Week", "variable":"Reporting Period", "modifiers":[{"variable":"Period Type", "value":"IsoWeek"}]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Period, Period type</t>
+      <t xml:space="preserve">]</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Period Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incidence rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">people/people</t>
+  </si>
+  <si>
     <t xml:space="preserve">[{"15 days Incidence rate":{"Variable":"Incidence Rate", "Calculation Period":"15 days"}}]</t>
   </si>
   <si>
     <t xml:space="preserve">Rt number</t>
   </si>
   <si>
-    <t xml:space="preserve">Calculation Period, Variant, Location, Pathogen, Period, Period type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of PPE Protective equipment</t>
   </si>
   <si>
@@ -183,9 +188,6 @@
     <t xml:space="preserve">Units/time</t>
   </si>
   <si>
-    <t xml:space="preserve">Location, Resource type, Unit, Pathogen, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Needs of PPE Protective equipment</t>
   </si>
   <si>
@@ -195,31 +197,41 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">Location, Pathogen, Period, Period type</t>
-  </si>
-  <si>
     <t xml:space="preserve">02. Deaths</t>
   </si>
   <si>
     <t xml:space="preserve">Number of deaths</t>
   </si>
   <si>
-    <t xml:space="preserve">Dead status, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Is Imported, Pathogen, Care facility, Eeference population, Period, Period type</t>
+    <t xml:space="preserve">reporting_period</t>
   </si>
   <si>
     <t xml:space="preserve">Mortality rates</t>
   </si>
   <si>
-    <t xml:space="preserve">Calculation period, Variant, Age, Age group, Gender, Comorbidity, Location, Pathogen, Care facility, External id, Period, Period type</t>
-  </si>
-  <si>
     <t xml:space="preserve">03. Patients</t>
   </si>
   <si>
     <t xml:space="preserve">Number of infected patients</t>
   </si>
   <si>
-    <t xml:space="preserve">Care facility, Care facility type, Bed type, Variant, Age, Age group, Gender, Comorbidity, Location, Severity Level, Patient Status, Treatment received,  Vaccination status, External id, Pathogen, Period, Period type</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reporting_period,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Severity</t>
+    </r>
   </si>
   <si>
     <r>
@@ -259,82 +271,49 @@
     <t xml:space="preserve">Number of non-infected patients </t>
   </si>
   <si>
-    <t xml:space="preserve">Care facility, Bed type, Vaccination status, External id, Reporting period, Pathogen, Period, Period type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Length of stay</t>
   </si>
   <si>
     <t xml:space="preserve">days</t>
   </si>
   <si>
-    <t xml:space="preserve">Care facility, External id, Pathogen, Period, Period type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of hospital staff</t>
   </si>
   <si>
-    <t xml:space="preserve">Stafff type, Staff subtype, Care facility, Pathogen vaccination status, Pathogen, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Qty of hospital resources</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Care facility, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of hospital resources dependencies</t>
   </si>
   <si>
-    <t xml:space="preserve">Base resource, reference resource, Care facility, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beds occupancy</t>
   </si>
   <si>
     <t xml:space="preserve">People</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource type, resource subtype,  Care facility, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">04.Tests</t>
   </si>
   <si>
     <t xml:space="preserve">Number of tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
-  </si>
-  <si>
     <t xml:space="preserve">Epidemiological surveys Answer</t>
   </si>
   <si>
-    <t xml:space="preserve">Epidemiological survey question, External Id, Test Result, Type of Test, Location, Period, External Id, Test Brand, Test Model, Reference population</t>
-  </si>
-  <si>
     <t xml:space="preserve">Positivity rate</t>
   </si>
   <si>
     <t xml:space="preserve">Number of test staff</t>
   </si>
   <si>
-    <t xml:space="preserve">Stafff type, Staff subtype, Test facility, Pathogen, Vaccination status, Pathogen, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Qty of test resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource type, resource subtype, Depletion mode, Test facility, Period</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of test resources dependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base resource, reference resource, Test facility, Period</t>
   </si>
   <si>
     <t xml:space="preserve">05. Vaccination</t>
@@ -637,7 +616,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -663,12 +642,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -748,13 +721,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -765,7 +738,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,1817 +784,1799 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="H37" s="1" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="H38" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>121</v>
+        <v>11</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>172</v>
+        <v>20</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H113"/>
+  <autoFilter ref="A1:H114">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Observation"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
fix issues writing to database
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -12,7 +12,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$H$115</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="170">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -68,7 +69,7 @@
     <t xml:space="preserve">reporting_period,case_status</t>
   </si>
   <si>
-    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]},{"alias":"Cases at onset of symptomps date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptomps date"}]}]</t>
+    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]}, {"alias":"Active cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Active"}]}, {"alias":"Reinfection cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Reinfection"}]}, {"alias":"Possible cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Possible"}]}, {"alias":"Probable cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Probable"}]}, {"alias":"Imported cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Imported"}]},{"alias":"Cases at onset of symptoms date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptoms date"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Pathogen Code</t>
@@ -523,6 +524,18 @@
   </si>
   <si>
     <t xml:space="preserve">Number detections variant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effective growth potential</t>
   </si>
 </sst>
 </file>
@@ -532,7 +545,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -553,6 +566,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -597,7 +618,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,6 +629,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -631,10 +656,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B101" activeCellId="0" sqref="B101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -646,7 +671,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="9" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -2495,6 +2521,71 @@
       <c r="H115" s="1" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H114"/>

</xml_diff>

<commit_message>
1. Changing Repeat implementation so it supports storing last execution 2. Implementing start and end hour for DLS (uising repeat) 3. Improving calculation of next execution in sources 4. Add a delay on standardize when a needed varuable is not yet published
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$115</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$115</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="165">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">Geo Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country code</t>
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Country Name", "variable":"Geo Name", "modifiers":[{"variable":"Geo Level", "value":"Country"}]}]</t>
@@ -633,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B101" activeCellId="0" sqref="B101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,10 +755,10 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,14 +766,14 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>17</v>
@@ -787,13 +784,13 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>17</v>
@@ -804,11 +801,11 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>17</v>
@@ -819,11 +816,11 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>17</v>
@@ -834,11 +831,11 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>17</v>
@@ -849,14 +846,14 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>17</v>
@@ -867,11 +864,11 @@
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>17</v>
@@ -882,14 +879,14 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,11 +894,11 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>17</v>
@@ -912,17 +909,17 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,14 +927,14 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>17</v>
@@ -948,14 +945,14 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
@@ -966,14 +963,14 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>17</v>
@@ -984,14 +981,14 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>17</v>
@@ -999,10 +996,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
@@ -1012,7 +1009,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
@@ -1020,17 +1017,17 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -1038,10 +1035,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
@@ -1051,22 +1048,22 @@
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>17</v>
@@ -1074,10 +1071,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -1092,17 +1089,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
@@ -1110,14 +1107,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -1128,17 +1125,17 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>17</v>
@@ -1146,17 +1143,17 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>17</v>
@@ -1164,17 +1161,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>17</v>
@@ -1182,17 +1179,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>17</v>
@@ -1200,17 +1197,17 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>17</v>
@@ -1218,17 +1215,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>17</v>
@@ -1236,14 +1233,14 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
@@ -1254,17 +1251,17 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>17</v>
@@ -1272,17 +1269,17 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>17</v>
@@ -1290,20 +1287,20 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>17</v>
@@ -1311,10 +1308,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
@@ -1324,18 +1321,18 @@
         <v>12</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
@@ -1347,14 +1344,14 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>17</v>
@@ -1362,14 +1359,14 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>17</v>
@@ -1377,14 +1374,14 @@
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>17</v>
@@ -1392,14 +1389,14 @@
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>17</v>
@@ -1407,14 +1404,14 @@
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>17</v>
@@ -1422,14 +1419,14 @@
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>17</v>
@@ -1437,14 +1434,14 @@
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>17</v>
@@ -1452,10 +1449,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
@@ -1467,14 +1464,14 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>17</v>
@@ -1482,14 +1479,14 @@
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>17</v>
@@ -1497,10 +1494,10 @@
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
@@ -1512,14 +1509,14 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>17</v>
@@ -1527,10 +1524,10 @@
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
@@ -1542,14 +1539,14 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>17</v>
@@ -1557,14 +1554,14 @@
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>17</v>
@@ -1572,14 +1569,14 @@
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>17</v>
@@ -1587,10 +1584,10 @@
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
@@ -1602,10 +1599,10 @@
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
@@ -1617,14 +1614,14 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>17</v>
@@ -1632,10 +1629,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
@@ -1647,14 +1644,14 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>17</v>
@@ -1662,14 +1659,14 @@
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>17</v>
@@ -1677,14 +1674,14 @@
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>17</v>
@@ -1692,14 +1689,14 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>17</v>
@@ -1707,10 +1704,10 @@
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
@@ -1722,10 +1719,10 @@
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
@@ -1737,14 +1734,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>17</v>
@@ -1752,10 +1749,10 @@
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
@@ -1767,14 +1764,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>17</v>
@@ -1782,10 +1779,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
@@ -1797,10 +1794,10 @@
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
@@ -1812,14 +1809,14 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>17</v>
@@ -1827,14 +1824,14 @@
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>17</v>
@@ -1842,14 +1839,14 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>17</v>
@@ -1857,10 +1854,10 @@
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
@@ -1872,10 +1869,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
@@ -1887,10 +1884,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
@@ -1902,14 +1899,14 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>17</v>
@@ -1917,14 +1914,14 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>17</v>
@@ -1932,14 +1929,14 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>17</v>
@@ -1947,14 +1944,14 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>17</v>
@@ -1962,14 +1959,14 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>17</v>
@@ -1977,10 +1974,10 @@
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
@@ -1992,10 +1989,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
@@ -2007,14 +2004,14 @@
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>17</v>
@@ -2022,14 +2019,14 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>17</v>
@@ -2037,10 +2034,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
@@ -2052,10 +2049,10 @@
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
@@ -2067,14 +2064,14 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>17</v>
@@ -2082,14 +2079,14 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
@@ -2097,14 +2094,14 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>17</v>
@@ -2112,14 +2109,14 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>17</v>
@@ -2127,14 +2124,14 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>17</v>
@@ -2142,14 +2139,14 @@
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>17</v>
@@ -2157,14 +2154,14 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>17</v>
@@ -2172,10 +2169,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
@@ -2187,14 +2184,14 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>17</v>
@@ -2205,7 +2202,7 @@
         <v>20</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
@@ -2220,7 +2217,7 @@
         <v>20</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
@@ -2235,7 +2232,7 @@
         <v>20</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
@@ -2250,7 +2247,7 @@
         <v>20</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
@@ -2265,7 +2262,7 @@
         <v>20</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
@@ -2280,7 +2277,7 @@
         <v>20</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
@@ -2295,7 +2292,7 @@
         <v>20</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
@@ -2305,7 +2302,7 @@
         <v>12</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>17</v>
@@ -2316,7 +2313,7 @@
         <v>20</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
@@ -2331,7 +2328,7 @@
         <v>20</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
@@ -2346,11 +2343,11 @@
         <v>20</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>17</v>
@@ -2361,11 +2358,11 @@
         <v>20</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>17</v>
@@ -2376,11 +2373,11 @@
         <v>20</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>17</v>
@@ -2388,10 +2385,10 @@
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
@@ -2403,10 +2400,10 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
@@ -2418,10 +2415,10 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
@@ -2433,10 +2430,10 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
@@ -2448,10 +2445,10 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
@@ -2463,10 +2460,10 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2" t="s">
@@ -2478,10 +2475,10 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -2490,14 +2487,14 @@
         <v>12</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H114"/>
+  <autoFilter ref="A1:H115"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
commit before merge of P2-42
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$114</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$119</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$H$115</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="180">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reporting Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">[{"alias":"Reporting Date", "variable":"Reporting period", "modifiers":[{"variable":"Period Type", "value":"Date"}]}, {"alias":"Reporting Week", "variable":"Reporting Period", "modifiers":[{"variable":"Period Type", "value":"IsoWeek"}]}]</t>
@@ -556,32 +559,7 @@
     <t xml:space="preserve">Number of events</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{"alias":"alerts on humans", "variable":"Number of alerts", "modifiers":[{"variable":"Alert topic", "value":"Potential case in humans"}]}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
+    <t xml:space="preserve">[{"alias":"alerts on humans", "variable":"Number of alerts", "modifiers":[{"variable":"Alert topic", "value":"Potential case in humans"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Number of alerts</t>
@@ -707,8 +685,8 @@
   </sheetPr>
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B124" activeCellId="0" sqref="B124"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H124" activeCellId="0" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,8 +941,11 @@
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,7 +953,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -987,17 +968,17 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,14 +986,14 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>17</v>
@@ -1023,14 +1004,14 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
@@ -1041,14 +1022,14 @@
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>17</v>
@@ -1059,14 +1040,14 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>17</v>
@@ -1074,10 +1055,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
@@ -1087,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
@@ -1095,17 +1076,17 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
@@ -1113,10 +1094,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
@@ -1126,18 +1107,18 @@
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
@@ -1149,10 +1130,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -1167,17 +1148,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
@@ -1185,14 +1166,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -1203,17 +1184,17 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>17</v>
@@ -1221,17 +1202,17 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>17</v>
@@ -1239,17 +1220,17 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>17</v>
@@ -1257,17 +1238,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>17</v>
@@ -1275,17 +1256,17 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>17</v>
@@ -1293,17 +1274,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>17</v>
@@ -1311,14 +1292,14 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
@@ -1329,17 +1310,17 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>17</v>
@@ -1347,17 +1328,17 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>17</v>
@@ -1365,20 +1346,20 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>17</v>
@@ -1386,10 +1367,10 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
@@ -1399,18 +1380,18 @@
         <v>12</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
@@ -1422,10 +1403,10 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
@@ -1437,10 +1418,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
@@ -1452,10 +1433,10 @@
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
@@ -1467,10 +1448,10 @@
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
@@ -1482,10 +1463,10 @@
     </row>
     <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
@@ -1497,14 +1478,14 @@
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>17</v>
@@ -1512,14 +1493,14 @@
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>17</v>
@@ -1527,10 +1508,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
@@ -1542,14 +1523,14 @@
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>17</v>
@@ -1557,10 +1538,10 @@
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
@@ -1572,10 +1553,10 @@
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
@@ -1587,10 +1568,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2" t="s">
@@ -1602,10 +1583,10 @@
     </row>
     <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2" t="s">
@@ -1617,10 +1598,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
@@ -1632,14 +1613,14 @@
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>17</v>
@@ -1647,14 +1628,14 @@
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>17</v>
@@ -1662,10 +1643,10 @@
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2" t="s">
@@ -1677,10 +1658,10 @@
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2" t="s">
@@ -1692,14 +1673,14 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>17</v>
@@ -1707,10 +1688,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2" t="s">
@@ -1722,10 +1703,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2" t="s">
@@ -1737,10 +1718,10 @@
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2" t="s">
@@ -1752,10 +1733,10 @@
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
@@ -1767,14 +1748,14 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>17</v>
@@ -1782,10 +1763,10 @@
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
@@ -1797,10 +1778,10 @@
     </row>
     <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2" t="s">
@@ -1812,10 +1793,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
@@ -1827,10 +1808,10 @@
     </row>
     <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
@@ -1842,10 +1823,10 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
@@ -1857,10 +1838,10 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
@@ -1872,10 +1853,10 @@
     </row>
     <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
@@ -1887,10 +1868,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
@@ -1902,14 +1883,14 @@
     </row>
     <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>17</v>
@@ -1917,14 +1898,14 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>17</v>
@@ -1932,10 +1913,10 @@
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2" t="s">
@@ -1947,10 +1928,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2" t="s">
@@ -1962,10 +1943,10 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2" t="s">
@@ -1977,10 +1958,10 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
@@ -1992,14 +1973,14 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>17</v>
@@ -2007,14 +1988,14 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>17</v>
@@ -2022,14 +2003,14 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>17</v>
@@ -2037,14 +2018,14 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>17</v>
@@ -2052,10 +2033,10 @@
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2" t="s">
@@ -2067,10 +2048,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
@@ -2082,10 +2063,10 @@
     </row>
     <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2" t="s">
@@ -2097,14 +2078,14 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>17</v>
@@ -2112,10 +2093,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
@@ -2127,10 +2108,10 @@
     </row>
     <row r="87" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
@@ -2142,14 +2123,14 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>17</v>
@@ -2157,14 +2138,14 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
@@ -2172,14 +2153,14 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>17</v>
@@ -2187,14 +2168,14 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>17</v>
@@ -2202,14 +2183,14 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>17</v>
@@ -2217,14 +2198,14 @@
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>17</v>
@@ -2232,14 +2213,14 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>17</v>
@@ -2247,10 +2228,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
@@ -2262,14 +2243,14 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>17</v>
@@ -2280,7 +2261,7 @@
         <v>20</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="2" t="s">
@@ -2295,7 +2276,7 @@
         <v>20</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
@@ -2310,7 +2291,7 @@
         <v>20</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
@@ -2325,7 +2306,7 @@
         <v>20</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2" t="s">
@@ -2340,7 +2321,7 @@
         <v>20</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="2" t="s">
@@ -2355,7 +2336,7 @@
         <v>20</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2" t="s">
@@ -2370,7 +2351,7 @@
         <v>20</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
@@ -2380,7 +2361,7 @@
         <v>12</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>17</v>
@@ -2391,7 +2372,7 @@
         <v>20</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="2" t="s">
@@ -2406,7 +2387,7 @@
         <v>20</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="2" t="s">
@@ -2421,11 +2402,11 @@
         <v>20</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>17</v>
@@ -2436,11 +2417,11 @@
         <v>20</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>17</v>
@@ -2451,11 +2432,11 @@
         <v>20</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>17</v>
@@ -2463,10 +2444,10 @@
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="2" t="s">
@@ -2478,10 +2459,10 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="2" t="s">
@@ -2493,10 +2474,10 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="2" t="s">
@@ -2508,10 +2489,10 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2" t="s">
@@ -2523,10 +2504,10 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
@@ -2538,10 +2519,10 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2" t="s">
@@ -2553,10 +2534,10 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>11</v>
@@ -2565,7 +2546,7 @@
         <v>12</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>17</v>
@@ -2576,7 +2557,7 @@
         <v>20</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>16</v>
@@ -2586,17 +2567,17 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>17</v>
@@ -2607,13 +2588,13 @@
         <v>20</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>17</v>
@@ -2624,13 +2605,13 @@
         <v>8</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>17</v>
@@ -2641,7 +2622,7 @@
         <v>8</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>11</v>
@@ -2655,7 +2636,7 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>11</v>
@@ -2665,25 +2646,49 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B122" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B123" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="B124" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H119"/>
+  <autoFilter ref="A1:H114"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Integrate local file acquisition with cases template
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="179">
   <si>
     <t xml:space="preserve">Data Family</t>
   </si>
@@ -66,10 +66,10 @@
     <t xml:space="preserve">people</t>
   </si>
   <si>
-    <t xml:space="preserve">reporting_period,case_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]}, {"alias":"Active cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Active"}]}, {"alias":"Reinfection cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Reinfection"}]}, {"alias":"Possible cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Possible"}]}, {"alias":"Probable cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Probable"}]}, {"alias":"Imported cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Imported"}]},{"alias":"Cases at onset of symptoms date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptoms date"}]}]</t>
+    <t xml:space="preserve">reporting_period,case_status,time_window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"alias":"Confirmed cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Confirmed"}]}, {"alias":"Recovered cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Recovered"}]}, {"alias":"Active cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Active"}]}, {"alias":"Reinfection cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Reinfection"}]}, {"alias":"Possible cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Possible"}]}, {"alias":"Probable cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Probable"}]}, {"alias":"Imported cases", "variable":"Number of Cases", "modifiers":[{"variable":"Case Status", "value":"Imported"}]},{"alias":"Cumulative cases", "variable":"Number of Cases", "modifiers":[{"variable":"Time window", "value":"Cumulative"}]}, {"alias":"Cases at onset of symptoms date", "variable":"Number of Cases", "modifiers":[{"variable":"period type", "value":"Onset of symptoms date"}]}]</t>
   </si>
   <si>
     <t xml:space="preserve">Pathogen Code</t>
@@ -532,7 +532,7 @@
     <t xml:space="preserve">Number detections variant</t>
   </si>
   <si>
-    <t xml:space="preserve">Gender</t>
+    <t xml:space="preserve">Gender code</t>
   </si>
   <si>
     <t xml:space="preserve">Gender name</t>
@@ -550,22 +550,19 @@
     <t xml:space="preserve">number</t>
   </si>
   <si>
-    <t xml:space="preserve">Alerts of potential cases in animals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alerts of potential cases in humans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"alias":"alerts on humans", "variable":"Number of alerts", "modifiers":[{"variable":"Alert topic", "value":"Potential case in humans"}]}]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of alerts</t>
   </si>
   <si>
+    <t xml:space="preserve">reporting_period,alert_topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{"alias":"alerts on humans", "variable":"Number of alerts", "modifiers":[{"variable":"Alert topic", "value":"Potential case in humans"}]}, {"alias":"alerts on animals", "variable":"Number of alerts", "modifiers":[{"variable":"Alert topic", "value":"Potential case in animals"}]}]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alert topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time window</t>
   </si>
 </sst>
 </file>
@@ -575,7 +572,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -596,11 +593,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -645,7 +637,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -656,10 +648,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -683,10 +671,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H124" activeCellId="0" sqref="H124"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2627,8 +2615,11 @@
       <c r="D120" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G120" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="H120" s="1" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2636,54 +2627,26 @@
         <v>8</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="s">
-        <v>8</v>
+      <c r="A122" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H123" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H124" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add incidence formula to the variables file
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="346">
   <si>
     <t xml:space="preserve">data_family</t>
   </si>
@@ -199,13 +199,16 @@
     <t xml:space="preserve">period_type</t>
   </si>
   <si>
-    <t xml:space="preserve">incidence_rate</t>
+    <t xml:space="preserve">incidence</t>
   </si>
   <si>
     <t xml:space="preserve">indicator</t>
   </si>
   <si>
     <t xml:space="preserve">ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indicence(reporting_period, number_of_cases, population)</t>
   </si>
   <si>
     <t xml:space="preserve">rt_number</t>
@@ -1178,8 +1181,8 @@
   </sheetPr>
   <dimension ref="A1:J227"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F192" activeCellId="0" sqref="F192"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1747,6 +1750,9 @@
       <c r="E28" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="H28" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="J28" s="0" t="s">
         <v>16</v>
       </c>
@@ -1756,13 +1762,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>16</v>
@@ -1773,13 +1779,13 @@
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J30" s="0" t="s">
         <v>16</v>
@@ -1790,13 +1796,13 @@
         <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>16</v>
@@ -1807,13 +1813,13 @@
         <v>10</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>16</v>
@@ -1821,10 +1827,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>13</v>
@@ -1841,10 +1847,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>13</v>
@@ -1856,7 +1862,7 @@
         <v>52</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>18</v>
@@ -1864,10 +1870,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>13</v>
@@ -1879,18 +1885,18 @@
         <v>52</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>13</v>
@@ -1902,18 +1908,18 @@
         <v>52</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>13</v>
@@ -1925,18 +1931,18 @@
         <v>52</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>44</v>
@@ -1947,16 +1953,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J39" s="0" t="s">
         <v>16</v>
@@ -1964,10 +1970,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>44</v>
@@ -1978,10 +1984,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>13</v>
@@ -1995,10 +2001,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>13</v>
@@ -2012,30 +2018,30 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="J43" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>13</v>
@@ -2044,18 +2050,18 @@
         <v>14</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>13</v>
@@ -2064,18 +2070,18 @@
         <v>14</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>13</v>
@@ -2084,18 +2090,18 @@
         <v>14</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>13</v>
@@ -2104,18 +2110,18 @@
         <v>14</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
@@ -2124,18 +2130,18 @@
         <v>14</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
@@ -2144,18 +2150,18 @@
         <v>14</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
@@ -2164,18 +2170,18 @@
         <v>14</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
@@ -2184,18 +2190,18 @@
         <v>14</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>44</v>
@@ -2206,10 +2212,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>44</v>
@@ -2220,10 +2226,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>13</v>
@@ -2234,16 +2240,16 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="J55" s="0" t="s">
         <v>18</v>
@@ -2251,10 +2257,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>60</v>
@@ -2265,33 +2271,33 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>60</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J58" s="0" t="s">
         <v>16</v>
@@ -2299,36 +2305,36 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="0" t="s">
+      <c r="I59" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="I59" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="J59" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J60" s="0" t="s">
         <v>16</v>
@@ -2336,13 +2342,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>14</v>
@@ -2353,16 +2359,16 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J62" s="0" t="s">
         <v>16</v>
@@ -2370,210 +2376,210 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I63" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="J63" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>44</v>
@@ -2584,10 +2590,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>44</v>
@@ -2598,10 +2604,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>44</v>
@@ -2612,16 +2618,16 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J76" s="0" t="s">
         <v>16</v>
@@ -2629,16 +2635,16 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J77" s="0" t="s">
         <v>16</v>
@@ -2646,13 +2652,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>14</v>
@@ -2663,19 +2669,19 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J79" s="0" t="s">
         <v>16</v>
@@ -2683,108 +2689,108 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G80" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="D80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="G80" s="0" t="s">
+      <c r="I80" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I80" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="J80" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G81" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I81" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I81" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="J81" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G82" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I82" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="J82" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G83" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I83" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I83" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="J83" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J84" s="0" t="s">
         <v>16</v>
@@ -2792,10 +2798,10 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>44</v>
@@ -2806,16 +2812,16 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J86" s="0" t="s">
         <v>16</v>
@@ -2823,16 +2829,16 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J87" s="0" t="s">
         <v>16</v>
@@ -2840,13 +2846,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>14</v>
@@ -2857,16 +2863,16 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J89" s="0" t="s">
         <v>16</v>
@@ -2874,16 +2880,16 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J90" s="0" t="s">
         <v>16</v>
@@ -2891,16 +2897,16 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G91" s="0" t="s">
         <v>52</v>
@@ -2911,10 +2917,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>13</v>
@@ -2923,7 +2929,7 @@
         <v>14</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J92" s="0" t="s">
         <v>16</v>
@@ -2931,33 +2937,33 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I93" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D93" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G93" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="I93" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="J93" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>13</v>
@@ -2966,21 +2972,21 @@
         <v>14</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>13</v>
@@ -2989,21 +2995,21 @@
         <v>14</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>13</v>
@@ -3012,21 +3018,21 @@
         <v>14</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>13</v>
@@ -3035,21 +3041,21 @@
         <v>14</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>13</v>
@@ -3058,21 +3064,21 @@
         <v>14</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>13</v>
@@ -3081,21 +3087,21 @@
         <v>14</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>13</v>
@@ -3104,21 +3110,21 @@
         <v>14</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>13</v>
@@ -3127,21 +3133,21 @@
         <v>14</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>13</v>
@@ -3150,21 +3156,21 @@
         <v>14</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>13</v>
@@ -3173,21 +3179,21 @@
         <v>14</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>13</v>
@@ -3196,21 +3202,21 @@
         <v>14</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>13</v>
@@ -3219,21 +3225,21 @@
         <v>14</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>13</v>
@@ -3242,21 +3248,21 @@
         <v>14</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>13</v>
@@ -3265,21 +3271,21 @@
         <v>14</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>13</v>
@@ -3288,21 +3294,21 @@
         <v>14</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>13</v>
@@ -3311,21 +3317,21 @@
         <v>14</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>44</v>
@@ -3336,10 +3342,10 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>44</v>
@@ -3350,10 +3356,10 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>44</v>
@@ -3364,10 +3370,10 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>13</v>
@@ -3378,10 +3384,10 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D114" s="0" t="s">
         <v>44</v>
@@ -3392,10 +3398,10 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>44</v>
@@ -3406,10 +3412,10 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>44</v>
@@ -3420,10 +3426,10 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>44</v>
@@ -3434,10 +3440,10 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>44</v>
@@ -3448,10 +3454,10 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>60</v>
@@ -3462,13 +3468,13 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J120" s="0" t="s">
         <v>16</v>
@@ -3476,10 +3482,10 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>13</v>
@@ -3490,10 +3496,10 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>13</v>
@@ -3504,146 +3510,146 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B123" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I123" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="D123" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I123" s="0" t="s">
-        <v>214</v>
-      </c>
       <c r="J123" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>44</v>
@@ -3654,10 +3660,10 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>44</v>
@@ -3668,10 +3674,10 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>44</v>
@@ -3682,10 +3688,10 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>44</v>
@@ -3696,10 +3702,10 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>34</v>
@@ -3710,10 +3716,10 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>60</v>
@@ -3724,10 +3730,10 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>60</v>
@@ -3738,10 +3744,10 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>44</v>
@@ -3752,10 +3758,10 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>13</v>
@@ -3766,10 +3772,10 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>44</v>
@@ -3780,10 +3786,10 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>13</v>
@@ -3794,10 +3800,10 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>44</v>
@@ -3808,10 +3814,10 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D143" s="0" t="s">
         <v>60</v>
@@ -3822,13 +3828,13 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>16</v>
@@ -3836,10 +3842,10 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D145" s="0" t="s">
         <v>13</v>
@@ -3850,10 +3856,10 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D146" s="0" t="s">
         <v>13</v>
@@ -3864,10 +3870,10 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D147" s="0" t="s">
         <v>60</v>
@@ -3878,10 +3884,10 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D148" s="0" t="s">
         <v>34</v>
@@ -3892,10 +3898,10 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D149" s="0" t="s">
         <v>13</v>
@@ -3906,10 +3912,10 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D150" s="0" t="s">
         <v>44</v>
@@ -3920,10 +3926,10 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D151" s="0" t="s">
         <v>44</v>
@@ -3934,10 +3940,10 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>44</v>
@@ -3948,13 +3954,13 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J153" s="0" t="s">
         <v>16</v>
@@ -3962,10 +3968,10 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D154" s="0" t="s">
         <v>13</v>
@@ -3976,10 +3982,10 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D155" s="0" t="s">
         <v>13</v>
@@ -3990,10 +3996,10 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D156" s="0" t="s">
         <v>44</v>
@@ -4004,10 +4010,10 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D157" s="0" t="s">
         <v>13</v>
@@ -4018,10 +4024,10 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D158" s="0" t="s">
         <v>44</v>
@@ -4032,10 +4038,10 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D159" s="0" t="s">
         <v>13</v>
@@ -4046,10 +4052,10 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D160" s="0" t="s">
         <v>13</v>
@@ -4060,10 +4066,10 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>44</v>
@@ -4074,13 +4080,13 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J162" s="0" t="s">
         <v>16</v>
@@ -4088,13 +4094,13 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J163" s="0" t="s">
         <v>16</v>
@@ -4102,10 +4108,10 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D164" s="0" t="s">
         <v>13</v>
@@ -4116,10 +4122,10 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D165" s="0" t="s">
         <v>13</v>
@@ -4130,10 +4136,10 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>13</v>
@@ -4144,10 +4150,10 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D167" s="0" t="s">
         <v>44</v>
@@ -4158,13 +4164,13 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>16</v>
@@ -4172,13 +4178,13 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J169" s="0" t="s">
         <v>16</v>
@@ -4186,13 +4192,13 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J170" s="0" t="s">
         <v>16</v>
@@ -4200,13 +4206,13 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J171" s="0" t="s">
         <v>16</v>
@@ -4214,10 +4220,10 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D172" s="0" t="s">
         <v>13</v>
@@ -4228,10 +4234,10 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>13</v>
@@ -4242,10 +4248,10 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>44</v>
@@ -4256,13 +4262,13 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J175" s="0" t="s">
         <v>16</v>
@@ -4270,10 +4276,10 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D176" s="0" t="s">
         <v>13</v>
@@ -4284,10 +4290,10 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
@@ -4298,10 +4304,10 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D178" s="0" t="s">
         <v>60</v>
@@ -4312,10 +4318,10 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D179" s="0" t="s">
         <v>60</v>
@@ -4326,10 +4332,10 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>60</v>
@@ -4340,10 +4346,10 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D181" s="0" t="s">
         <v>60</v>
@@ -4354,10 +4360,10 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D182" s="0" t="s">
         <v>60</v>
@@ -4368,10 +4374,10 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>60</v>
@@ -4382,10 +4388,10 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>60</v>
@@ -4396,10 +4402,10 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D185" s="0" t="s">
         <v>13</v>
@@ -4410,13 +4416,13 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J186" s="0" t="s">
         <v>16</v>
@@ -4427,7 +4433,7 @@
         <v>37</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>34</v>
@@ -4441,7 +4447,7 @@
         <v>37</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>34</v>
@@ -4455,7 +4461,7 @@
         <v>37</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>34</v>
@@ -4469,7 +4475,7 @@
         <v>37</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>34</v>
@@ -4483,7 +4489,7 @@
         <v>37</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>34</v>
@@ -4497,13 +4503,13 @@
         <v>37</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D192" s="0" t="s">
         <v>36</v>
       </c>
       <c r="F192" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="J192" s="0" t="s">
         <v>16</v>
@@ -4514,7 +4520,7 @@
         <v>37</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>13</v>
@@ -4531,7 +4537,7 @@
         <v>37</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>13</v>
@@ -4545,7 +4551,7 @@
         <v>37</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>34</v>
@@ -4559,7 +4565,7 @@
         <v>37</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>13</v>
@@ -4579,7 +4585,7 @@
         <v>37</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>34</v>
@@ -4593,7 +4599,7 @@
         <v>37</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>34</v>
@@ -4607,10 +4613,10 @@
         <v>37</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J199" s="0" t="s">
         <v>16</v>
@@ -4621,10 +4627,10 @@
         <v>37</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J200" s="0" t="s">
         <v>16</v>
@@ -4635,10 +4641,10 @@
         <v>37</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J201" s="0" t="s">
         <v>16</v>
@@ -4646,10 +4652,10 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>34</v>
@@ -4660,10 +4666,10 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>34</v>
@@ -4674,10 +4680,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>34</v>
@@ -4688,10 +4694,10 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>34</v>
@@ -4702,10 +4708,10 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>34</v>
@@ -4716,10 +4722,10 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>34</v>
@@ -4730,10 +4736,10 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>13</v>
@@ -4753,7 +4759,7 @@
         <v>37</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>34</v>
@@ -4767,13 +4773,13 @@
         <v>37</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>36</v>
       </c>
       <c r="F210" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="J210" s="0" t="s">
         <v>16</v>
@@ -4784,13 +4790,13 @@
         <v>37</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D211" s="0" t="s">
         <v>34</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="J211" s="0" t="s">
         <v>16</v>
@@ -4801,13 +4807,13 @@
         <v>10</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D212" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J212" s="0" t="s">
         <v>16</v>
@@ -4818,13 +4824,13 @@
         <v>10</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G213" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J213" s="0" t="s">
         <v>16</v>
@@ -4835,19 +4841,19 @@
         <v>10</v>
       </c>
       <c r="B214" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D214" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G214" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="D214" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G214" s="0" t="s">
+      <c r="I214" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="I214" s="0" t="s">
-        <v>324</v>
-      </c>
       <c r="J214" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4855,19 +4861,19 @@
         <v>10</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G215" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="I215" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="I215" s="0" t="s">
-        <v>324</v>
-      </c>
       <c r="J215" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,7 +4881,7 @@
         <v>10</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D216" s="0" t="s">
         <v>44</v>
@@ -4889,7 +4895,7 @@
         <v>10</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D217" s="0" t="s">
         <v>13</v>
@@ -4906,19 +4912,19 @@
         <v>10</v>
       </c>
       <c r="B218" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I218" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="D218" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E218" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I218" s="0" t="s">
-        <v>331</v>
-      </c>
       <c r="J218" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,7 +4932,7 @@
         <v>10</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>13</v>
@@ -4935,10 +4941,10 @@
         <v>14</v>
       </c>
       <c r="I219" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J219" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4946,7 +4952,7 @@
         <v>10</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>13</v>
@@ -4955,10 +4961,10 @@
         <v>14</v>
       </c>
       <c r="I220" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4966,7 +4972,7 @@
         <v>10</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>13</v>
@@ -4975,10 +4981,10 @@
         <v>14</v>
       </c>
       <c r="I221" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J221" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,7 +4992,7 @@
         <v>10</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>60</v>
@@ -5000,7 +5006,7 @@
         <v>10</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D223" s="0" t="s">
         <v>60</v>
@@ -5014,7 +5020,7 @@
         <v>10</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D224" s="0" t="s">
         <v>34</v>
@@ -5028,7 +5034,7 @@
         <v>10</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>34</v>
@@ -5039,10 +5045,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>34</v>
@@ -5053,10 +5059,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
First commit for indicators calculation
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="348">
   <si>
     <t xml:space="preserve">data_family</t>
   </si>
@@ -166,6 +166,9 @@
     <t xml:space="preserve">source</t>
   </si>
   <si>
+    <t xml:space="preserve">not_characteristic</t>
+  </si>
+  <si>
     <t xml:space="preserve">file</t>
   </si>
   <si>
@@ -208,7 +211,7 @@
     <t xml:space="preserve">ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">indicence(reporting_period, number_of_cases, population)</t>
+    <t xml:space="preserve">incidence(reporting_period, number_of_cases, population)</t>
   </si>
   <si>
     <t xml:space="preserve">rt_number</t>
@@ -1041,6 +1044,9 @@
   </si>
   <si>
     <t xml:space="preserve">[{'variable': 'patient_status', 'value': 'sari'}, {'variable': 'response_status', 'value': 'hospitalised'}, {'variable': 'case_status', 'value': 'confirmed'}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response_status</t>
   </si>
   <si>
     <t xml:space="preserve">positivity_for_influenza_ari_ili</t>
@@ -1179,20 +1185,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J227"/>
+  <dimension ref="A1:J228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="40.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.12"/>
   </cols>
@@ -1593,7 +1601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>37</v>
       </c>
@@ -1601,35 +1609,35 @@
         <v>47</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="J20" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>16</v>
@@ -1640,7 +1648,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>44</v>
@@ -1657,7 +1665,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>44</v>
@@ -1671,13 +1679,13 @@
         <v>37</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>16</v>
@@ -1688,19 +1696,19 @@
         <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="J25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,19 +1716,19 @@
         <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="J26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,7 +1736,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>44</v>
@@ -1742,16 +1750,16 @@
         <v>10</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>16</v>
@@ -1762,13 +1770,13 @@
         <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>16</v>
@@ -1779,13 +1787,13 @@
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J30" s="0" t="s">
         <v>16</v>
@@ -1796,13 +1804,13 @@
         <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>16</v>
@@ -1813,13 +1821,13 @@
         <v>10</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>16</v>
@@ -1827,10 +1835,10 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>13</v>
@@ -1839,7 +1847,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>16</v>
@@ -1847,22 +1855,22 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B34" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I34" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>18</v>
@@ -1870,10 +1878,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>13</v>
@@ -1882,21 +1890,21 @@
         <v>14</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>13</v>
@@ -1905,21 +1913,21 @@
         <v>14</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>13</v>
@@ -1928,21 +1936,21 @@
         <v>14</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>44</v>
@@ -1953,16 +1961,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J39" s="0" t="s">
         <v>16</v>
@@ -1970,10 +1978,10 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>44</v>
@@ -1984,10 +1992,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>13</v>
@@ -2001,10 +2009,10 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>13</v>
@@ -2018,30 +2026,30 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="J43" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>13</v>
@@ -2050,18 +2058,18 @@
         <v>14</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>13</v>
@@ -2070,18 +2078,18 @@
         <v>14</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>13</v>
@@ -2090,18 +2098,18 @@
         <v>14</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>13</v>
@@ -2110,18 +2118,18 @@
         <v>14</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
@@ -2130,18 +2138,18 @@
         <v>14</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
@@ -2150,18 +2158,18 @@
         <v>14</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
@@ -2170,18 +2178,18 @@
         <v>14</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
@@ -2190,18 +2198,18 @@
         <v>14</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>44</v>
@@ -2212,10 +2220,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>44</v>
@@ -2226,10 +2234,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>13</v>
@@ -2240,16 +2248,16 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="J55" s="0" t="s">
         <v>18</v>
@@ -2257,13 +2265,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J56" s="0" t="s">
         <v>16</v>
@@ -2271,33 +2279,33 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>110</v>
-      </c>
       <c r="J57" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J58" s="0" t="s">
         <v>16</v>
@@ -2305,36 +2313,36 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B59" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="0" t="s">
+      <c r="I59" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="I59" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="J59" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J60" s="0" t="s">
         <v>16</v>
@@ -2342,13 +2350,13 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>14</v>
@@ -2359,16 +2367,16 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J62" s="0" t="s">
         <v>16</v>
@@ -2376,210 +2384,210 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I63" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="J63" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>44</v>
@@ -2590,10 +2598,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>44</v>
@@ -2604,10 +2612,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>44</v>
@@ -2618,16 +2626,16 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J76" s="0" t="s">
         <v>16</v>
@@ -2635,16 +2643,16 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J77" s="0" t="s">
         <v>16</v>
@@ -2652,13 +2660,13 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>14</v>
@@ -2669,19 +2677,19 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J79" s="0" t="s">
         <v>16</v>
@@ -2689,108 +2697,108 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G80" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G80" s="0" t="s">
+      <c r="I80" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I80" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="J80" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G81" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I81" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I81" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="J81" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G82" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I82" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I82" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="J82" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G83" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I83" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I83" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="J83" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J84" s="0" t="s">
         <v>16</v>
@@ -2798,10 +2806,10 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>44</v>
@@ -2812,16 +2820,16 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J86" s="0" t="s">
         <v>16</v>
@@ -2829,16 +2837,16 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J87" s="0" t="s">
         <v>16</v>
@@ -2846,13 +2854,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>14</v>
@@ -2863,16 +2871,16 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J89" s="0" t="s">
         <v>16</v>
@@ -2880,16 +2888,16 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J90" s="0" t="s">
         <v>16</v>
@@ -2897,19 +2905,19 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J91" s="0" t="s">
         <v>16</v>
@@ -2917,10 +2925,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>13</v>
@@ -2929,7 +2937,7 @@
         <v>14</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J92" s="0" t="s">
         <v>16</v>
@@ -2937,33 +2945,33 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="I93" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="D93" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G93" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="I93" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="J93" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>13</v>
@@ -2972,21 +2980,21 @@
         <v>14</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>13</v>
@@ -2995,21 +3003,21 @@
         <v>14</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>13</v>
@@ -3018,21 +3026,21 @@
         <v>14</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>13</v>
@@ -3041,21 +3049,21 @@
         <v>14</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>13</v>
@@ -3064,21 +3072,21 @@
         <v>14</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>13</v>
@@ -3087,21 +3095,21 @@
         <v>14</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>13</v>
@@ -3110,21 +3118,21 @@
         <v>14</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>13</v>
@@ -3133,21 +3141,21 @@
         <v>14</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>13</v>
@@ -3156,21 +3164,21 @@
         <v>14</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>13</v>
@@ -3179,21 +3187,21 @@
         <v>14</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>13</v>
@@ -3202,21 +3210,21 @@
         <v>14</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>13</v>
@@ -3225,21 +3233,21 @@
         <v>14</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>13</v>
@@ -3248,21 +3256,21 @@
         <v>14</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>13</v>
@@ -3271,21 +3279,21 @@
         <v>14</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>13</v>
@@ -3294,21 +3302,21 @@
         <v>14</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>13</v>
@@ -3317,21 +3325,21 @@
         <v>14</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>44</v>
@@ -3342,10 +3350,10 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>44</v>
@@ -3356,10 +3364,10 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>44</v>
@@ -3370,10 +3378,10 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>13</v>
@@ -3384,10 +3392,10 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D114" s="0" t="s">
         <v>44</v>
@@ -3398,10 +3406,10 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>44</v>
@@ -3412,10 +3420,10 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>44</v>
@@ -3426,10 +3434,10 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>44</v>
@@ -3440,10 +3448,10 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>44</v>
@@ -3454,13 +3462,13 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J119" s="0" t="s">
         <v>16</v>
@@ -3468,13 +3476,13 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J120" s="0" t="s">
         <v>16</v>
@@ -3482,10 +3490,10 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>13</v>
@@ -3496,10 +3504,10 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>13</v>
@@ -3510,146 +3518,146 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B123" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I123" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="D123" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I123" s="0" t="s">
-        <v>215</v>
-      </c>
       <c r="J123" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>44</v>
@@ -3660,10 +3668,10 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>44</v>
@@ -3674,10 +3682,10 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>44</v>
@@ -3688,10 +3696,10 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>44</v>
@@ -3702,10 +3710,10 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>34</v>
@@ -3716,13 +3724,13 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J136" s="0" t="s">
         <v>16</v>
@@ -3730,13 +3738,13 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J137" s="0" t="s">
         <v>16</v>
@@ -3744,10 +3752,10 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>44</v>
@@ -3758,10 +3766,10 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>13</v>
@@ -3772,10 +3780,10 @@
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>44</v>
@@ -3786,10 +3794,10 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>13</v>
@@ -3800,10 +3808,10 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>44</v>
@@ -3814,13 +3822,13 @@
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J143" s="0" t="s">
         <v>16</v>
@@ -3828,13 +3836,13 @@
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>16</v>
@@ -3842,10 +3850,10 @@
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D145" s="0" t="s">
         <v>13</v>
@@ -3856,10 +3864,10 @@
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D146" s="0" t="s">
         <v>13</v>
@@ -3870,13 +3878,13 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J147" s="0" t="s">
         <v>16</v>
@@ -3884,10 +3892,10 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D148" s="0" t="s">
         <v>34</v>
@@ -3898,10 +3906,10 @@
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D149" s="0" t="s">
         <v>13</v>
@@ -3912,10 +3920,10 @@
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D150" s="0" t="s">
         <v>44</v>
@@ -3926,10 +3934,10 @@
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D151" s="0" t="s">
         <v>44</v>
@@ -3940,10 +3948,10 @@
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>44</v>
@@ -3954,13 +3962,13 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J153" s="0" t="s">
         <v>16</v>
@@ -3968,10 +3976,10 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D154" s="0" t="s">
         <v>13</v>
@@ -3982,10 +3990,10 @@
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D155" s="0" t="s">
         <v>13</v>
@@ -3996,10 +4004,10 @@
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D156" s="0" t="s">
         <v>44</v>
@@ -4010,10 +4018,10 @@
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D157" s="0" t="s">
         <v>13</v>
@@ -4024,10 +4032,10 @@
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D158" s="0" t="s">
         <v>44</v>
@@ -4038,10 +4046,10 @@
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D159" s="0" t="s">
         <v>13</v>
@@ -4052,10 +4060,10 @@
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D160" s="0" t="s">
         <v>13</v>
@@ -4066,10 +4074,10 @@
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>44</v>
@@ -4080,13 +4088,13 @@
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J162" s="0" t="s">
         <v>16</v>
@@ -4094,13 +4102,13 @@
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J163" s="0" t="s">
         <v>16</v>
@@ -4108,10 +4116,10 @@
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D164" s="0" t="s">
         <v>13</v>
@@ -4122,10 +4130,10 @@
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D165" s="0" t="s">
         <v>13</v>
@@ -4136,10 +4144,10 @@
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>13</v>
@@ -4150,10 +4158,10 @@
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D167" s="0" t="s">
         <v>44</v>
@@ -4164,13 +4172,13 @@
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>16</v>
@@ -4178,13 +4186,13 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J169" s="0" t="s">
         <v>16</v>
@@ -4192,13 +4200,13 @@
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J170" s="0" t="s">
         <v>16</v>
@@ -4206,13 +4214,13 @@
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J171" s="0" t="s">
         <v>16</v>
@@ -4220,10 +4228,10 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D172" s="0" t="s">
         <v>13</v>
@@ -4234,10 +4242,10 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>13</v>
@@ -4248,10 +4256,10 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>44</v>
@@ -4262,13 +4270,13 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J175" s="0" t="s">
         <v>16</v>
@@ -4276,10 +4284,10 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D176" s="0" t="s">
         <v>13</v>
@@ -4290,10 +4298,10 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
@@ -4304,13 +4312,13 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J178" s="0" t="s">
         <v>16</v>
@@ -4318,13 +4326,13 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J179" s="0" t="s">
         <v>16</v>
@@ -4332,13 +4340,13 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J180" s="0" t="s">
         <v>16</v>
@@ -4346,13 +4354,13 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J181" s="0" t="s">
         <v>16</v>
@@ -4360,13 +4368,13 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J182" s="0" t="s">
         <v>16</v>
@@ -4374,13 +4382,13 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J183" s="0" t="s">
         <v>16</v>
@@ -4388,13 +4396,13 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J184" s="0" t="s">
         <v>16</v>
@@ -4402,10 +4410,10 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D185" s="0" t="s">
         <v>13</v>
@@ -4416,13 +4424,13 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J186" s="0" t="s">
         <v>16</v>
@@ -4433,7 +4441,7 @@
         <v>37</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>34</v>
@@ -4447,7 +4455,7 @@
         <v>37</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>34</v>
@@ -4461,7 +4469,7 @@
         <v>37</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>34</v>
@@ -4475,7 +4483,7 @@
         <v>37</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>34</v>
@@ -4489,7 +4497,7 @@
         <v>37</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>34</v>
@@ -4503,13 +4511,13 @@
         <v>37</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D192" s="0" t="s">
         <v>36</v>
       </c>
       <c r="F192" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="J192" s="0" t="s">
         <v>16</v>
@@ -4520,13 +4528,13 @@
         <v>37</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E193" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J193" s="0" t="s">
         <v>16</v>
@@ -4537,7 +4545,7 @@
         <v>37</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>13</v>
@@ -4551,7 +4559,7 @@
         <v>37</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>34</v>
@@ -4565,7 +4573,7 @@
         <v>37</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>13</v>
@@ -4574,7 +4582,7 @@
         <v>14</v>
       </c>
       <c r="G196" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J196" s="0" t="s">
         <v>16</v>
@@ -4585,7 +4593,7 @@
         <v>37</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>34</v>
@@ -4599,7 +4607,7 @@
         <v>37</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>34</v>
@@ -4613,10 +4621,10 @@
         <v>37</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J199" s="0" t="s">
         <v>16</v>
@@ -4627,10 +4635,10 @@
         <v>37</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J200" s="0" t="s">
         <v>16</v>
@@ -4641,10 +4649,10 @@
         <v>37</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J201" s="0" t="s">
         <v>16</v>
@@ -4652,10 +4660,10 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>34</v>
@@ -4666,10 +4674,10 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>34</v>
@@ -4680,10 +4688,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>34</v>
@@ -4694,10 +4702,10 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>34</v>
@@ -4708,10 +4716,10 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>34</v>
@@ -4722,10 +4730,10 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>34</v>
@@ -4736,10 +4744,10 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>13</v>
@@ -4748,7 +4756,7 @@
         <v>14</v>
       </c>
       <c r="G208" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J208" s="0" t="s">
         <v>16</v>
@@ -4759,7 +4767,7 @@
         <v>37</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>34</v>
@@ -4773,13 +4781,13 @@
         <v>37</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>36</v>
       </c>
       <c r="F210" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="J210" s="0" t="s">
         <v>16</v>
@@ -4790,13 +4798,13 @@
         <v>37</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D211" s="0" t="s">
         <v>34</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="J211" s="0" t="s">
         <v>16</v>
@@ -4807,13 +4815,13 @@
         <v>10</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="J212" s="0" t="s">
         <v>16</v>
@@ -4824,13 +4832,13 @@
         <v>10</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G213" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J213" s="0" t="s">
         <v>16</v>
@@ -4841,19 +4849,19 @@
         <v>10</v>
       </c>
       <c r="B214" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="D214" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G214" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="D214" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G214" s="0" t="s">
+      <c r="I214" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="I214" s="0" t="s">
-        <v>325</v>
-      </c>
       <c r="J214" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4861,19 +4869,19 @@
         <v>10</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G215" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="I215" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="I215" s="0" t="s">
-        <v>325</v>
-      </c>
       <c r="J215" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4881,7 +4889,7 @@
         <v>10</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D216" s="0" t="s">
         <v>44</v>
@@ -4895,7 +4903,7 @@
         <v>10</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D217" s="0" t="s">
         <v>13</v>
@@ -4912,19 +4920,19 @@
         <v>10</v>
       </c>
       <c r="B218" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I218" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="D218" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E218" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I218" s="0" t="s">
-        <v>332</v>
-      </c>
       <c r="J218" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4932,7 +4940,7 @@
         <v>10</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>13</v>
@@ -4941,10 +4949,10 @@
         <v>14</v>
       </c>
       <c r="I219" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J219" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4952,7 +4960,7 @@
         <v>10</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>13</v>
@@ -4961,18 +4969,18 @@
         <v>14</v>
       </c>
       <c r="I220" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>13</v>
@@ -4981,21 +4989,21 @@
         <v>14</v>
       </c>
       <c r="I221" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J221" s="0" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="J222" s="0" t="s">
         <v>16</v>
@@ -5006,10 +5014,10 @@
         <v>10</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J223" s="0" t="s">
         <v>16</v>
@@ -5020,10 +5028,10 @@
         <v>10</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="J224" s="0" t="s">
         <v>16</v>
@@ -5034,7 +5042,7 @@
         <v>10</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>34</v>
@@ -5045,10 +5053,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>34</v>
@@ -5059,15 +5067,29 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>34</v>
       </c>
       <c r="J227" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J228" s="0" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding RIVM dedicated template and fixing errors for publication
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$228</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="348">
   <si>
     <t xml:space="preserve">data_family</t>
   </si>
@@ -139,6 +142,9 @@
     <t xml:space="preserve">geo_code</t>
   </si>
   <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
     <t xml:space="preserve">iso_country_code_2</t>
   </si>
   <si>
@@ -163,7 +169,7 @@
     <t xml:space="preserve">Country, NUTS_1, NUTS_2, NUTS_3</t>
   </si>
   <si>
-    <t xml:space="preserve">source</t>
+    <t xml:space="preserve">geo_local_code</t>
   </si>
   <si>
     <t xml:space="preserve">file</t>
@@ -220,7 +226,7 @@
     <t xml:space="preserve">number_of_ppe_protective_equipment</t>
   </si>
   <si>
-    <t xml:space="preserve">resources</t>
+    <t xml:space="preserve">resource</t>
   </si>
   <si>
     <t xml:space="preserve">units/time</t>
@@ -286,6 +292,9 @@
     <t xml:space="preserve">number_of_patients</t>
   </si>
   <si>
+    <t xml:space="preserve">reporting_period, care_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">hospitalised_infected_patients</t>
   </si>
   <si>
@@ -376,6 +385,9 @@
     <t xml:space="preserve">number_of_hospital_staff</t>
   </si>
   <si>
+    <t xml:space="preserve">reporting_period, source</t>
+  </si>
+  <si>
     <t xml:space="preserve">number_of_resources</t>
   </si>
   <si>
@@ -461,9 +473,6 @@
   </si>
   <si>
     <t xml:space="preserve">performed_tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reporting_period, source</t>
   </si>
   <si>
     <t xml:space="preserve">positive_results</t>
@@ -1068,7 +1077,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1098,6 +1107,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1149,13 +1164,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1174,25 +1193,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J227"/>
+  <dimension ref="A1:J228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="40.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.12"/>
   </cols>
@@ -1491,7 +1516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>37</v>
       </c>
@@ -1501,33 +1526,39 @@
       <c r="D13" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="G13" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="J13" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="G14" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="I14" s="0" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>36</v>
@@ -1535,16 +1566,19 @@
       <c r="F15" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="G15" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="J15" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>36</v>
@@ -1552,56 +1586,71 @@
       <c r="F16" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="G16" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="I16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="G17" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="J17" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>44</v>
+      <c r="G18" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>16</v>
@@ -1612,10 +1661,10 @@
         <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>16</v>
@@ -1629,7 +1678,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>16</v>
@@ -1643,10 +1692,7 @@
         <v>50</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>16</v>
@@ -1654,13 +1700,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>51</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>16</v>
@@ -1668,16 +1717,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>16</v>
@@ -1688,19 +1734,16 @@
         <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="J25" s="0" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,19 +1751,19 @@
         <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,30 +1771,30 @@
         <v>37</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>16</v>
@@ -1762,13 +1805,16 @@
         <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>16</v>
@@ -1779,36 +1825,36 @@
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="J30" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="J31" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>10</v>
       </c>
@@ -1816,38 +1862,35 @@
         <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="J32" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="J33" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>73</v>
@@ -1859,18 +1902,15 @@
         <v>14</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>74</v>
@@ -1882,21 +1922,21 @@
         <v>14</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="B36" s="0" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>13</v>
@@ -1905,21 +1945,21 @@
         <v>14</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I36" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="B37" s="0" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>13</v>
@@ -1928,80 +1968,86 @@
         <v>14</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="B38" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="D38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J38" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="0" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>82</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="J39" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="D40" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="J40" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>86</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J41" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>87</v>
@@ -2016,9 +2062,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>88</v>
@@ -2029,19 +2075,19 @@
       <c r="E43" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="0" t="s">
-        <v>87</v>
+      <c r="G43" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>13</v>
@@ -2049,19 +2095,22 @@
       <c r="E44" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G44" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>13</v>
@@ -2069,16 +2118,19 @@
       <c r="E45" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G45" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I45" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>92</v>
@@ -2089,16 +2141,19 @@
       <c r="E46" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G46" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I46" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J46" s="0" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>94</v>
@@ -2109,16 +2164,19 @@
       <c r="E47" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G47" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I47" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J47" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>96</v>
@@ -2129,16 +2187,19 @@
       <c r="E48" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G48" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J48" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>98</v>
@@ -2149,16 +2210,19 @@
       <c r="E49" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G49" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I49" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J49" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>100</v>
@@ -2169,16 +2233,19 @@
       <c r="E50" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G50" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I50" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J50" s="0" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>102</v>
@@ -2189,28 +2256,40 @@
       <c r="E51" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G51" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="I51" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J51" s="0" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="D52" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="J52" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>106</v>
       </c>
@@ -2218,94 +2297,91 @@
         <v>107</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J53" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J54" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="J55" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="J56" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J58" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="J58" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>115</v>
@@ -2314,405 +2390,435 @@
         <v>13</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>114</v>
+      <c r="I60" s="0" t="s">
+        <v>115</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E61" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="J61" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>64</v>
+      <c r="G62" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="J62" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>118</v>
+        <v>65</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="J63" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G64" s="0" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B64" s="0" t="s">
+      <c r="I64" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>118</v>
-      </c>
       <c r="J64" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>121</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>106</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J74" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J75" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E76" s="0" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J76" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J77" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E78" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E79" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="J78" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G79" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="J79" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E80" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="I80" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="J80" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>150</v>
@@ -2721,21 +2827,21 @@
         <v>13</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J81" s="0" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>152</v>
@@ -2744,21 +2850,21 @@
         <v>13</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J82" s="0" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>154</v>
@@ -2767,180 +2873,183 @@
         <v>13</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I83" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J83" s="0" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="D84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="J84" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J84" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="J85" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J86" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="J87" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E88" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E89" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="J88" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E89" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="J89" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J90" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>165</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G91" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="J91" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B92" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D92" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G92" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="J92" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>164</v>
-      </c>
       <c r="B93" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>13</v>
@@ -2949,18 +3058,15 @@
         <v>14</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="I93" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J93" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="J93" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>164</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>169</v>
@@ -2972,10 +3078,10 @@
         <v>14</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J94" s="0" t="s">
         <v>170</v>
@@ -2983,7 +3089,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>171</v>
@@ -2995,10 +3101,10 @@
         <v>14</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J95" s="0" t="s">
         <v>172</v>
@@ -3006,7 +3112,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>173</v>
@@ -3018,10 +3124,10 @@
         <v>14</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J96" s="0" t="s">
         <v>174</v>
@@ -3029,7 +3135,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>175</v>
@@ -3041,18 +3147,18 @@
         <v>14</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J97" s="0" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>177</v>
@@ -3064,18 +3170,18 @@
         <v>14</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J98" s="0" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>179</v>
@@ -3087,18 +3193,18 @@
         <v>14</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J99" s="0" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>181</v>
@@ -3110,18 +3216,18 @@
         <v>14</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J100" s="0" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>183</v>
@@ -3133,18 +3239,18 @@
         <v>14</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J101" s="0" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>185</v>
@@ -3156,18 +3262,18 @@
         <v>14</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J102" s="0" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>187</v>
@@ -3179,18 +3285,18 @@
         <v>14</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J103" s="0" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>189</v>
@@ -3202,18 +3308,18 @@
         <v>14</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J104" s="0" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>191</v>
@@ -3225,18 +3331,18 @@
         <v>14</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J105" s="0" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>193</v>
@@ -3248,18 +3354,18 @@
         <v>14</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J106" s="0" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>195</v>
@@ -3271,18 +3377,18 @@
         <v>14</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J107" s="0" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>197</v>
@@ -3294,18 +3400,18 @@
         <v>14</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J108" s="0" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>199</v>
@@ -3317,217 +3423,223 @@
         <v>14</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J109" s="0" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>201</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I110" s="0" t="s">
+        <v>168</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>203</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J111" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>164</v>
+        <v>204</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J112" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J113" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J114" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J115" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J116" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J117" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J118" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="J119" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J120" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>213</v>
+        <v>166</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>214</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="J121" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B122" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J122" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="D122" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J122" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
-        <v>213</v>
-      </c>
       <c r="B123" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I123" s="0" t="s">
+      <c r="J123" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="J123" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
-        <v>213</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>218</v>
@@ -3536,15 +3648,15 @@
         <v>13</v>
       </c>
       <c r="I124" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J124" s="0" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>220</v>
@@ -3553,15 +3665,15 @@
         <v>13</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J125" s="0" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>222</v>
@@ -3570,15 +3682,15 @@
         <v>13</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J126" s="0" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>224</v>
@@ -3587,15 +3699,15 @@
         <v>13</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J127" s="0" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>226</v>
@@ -3604,15 +3716,15 @@
         <v>13</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J128" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>228</v>
@@ -3621,15 +3733,15 @@
         <v>13</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J129" s="0" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>230</v>
@@ -3638,508 +3750,511 @@
         <v>13</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J130" s="0" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>232</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>217</v>
       </c>
       <c r="J131" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J132" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J133" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J134" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D135" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J135" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="D136" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J135" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B136" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="D136" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="J136" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J137" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="J138" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J139" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J140" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J141" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J142" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="J143" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="B145" s="0" t="s">
         <v>247</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="J145" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B146" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D146" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J146" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="D146" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J146" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
-        <v>246</v>
-      </c>
       <c r="B147" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="J147" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D148" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J148" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="D149" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J148" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="B149" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="D149" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="J149" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J150" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J151" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J152" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="J153" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B154" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B154" s="0" t="s">
+      <c r="D154" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="D154" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="J154" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B155" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J155" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="D155" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J155" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
-        <v>257</v>
-      </c>
       <c r="B156" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J156" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J157" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J158" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B159" s="0" t="s">
         <v>264</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J159" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B160" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J160" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="D160" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J160" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
-        <v>263</v>
-      </c>
       <c r="B161" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J161" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="J162" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D163" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J163" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>270</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="J164" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B165" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J165" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="D165" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J165" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
-        <v>269</v>
-      </c>
       <c r="B166" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>13</v>
@@ -4148,71 +4263,71 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J167" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J169" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J170" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>256</v>
+        <v>67</v>
       </c>
       <c r="J171" s="0" t="s">
         <v>16</v>
@@ -4220,13 +4335,13 @@
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>279</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="J172" s="0" t="s">
         <v>16</v>
@@ -4234,10 +4349,10 @@
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>13</v>
@@ -4248,13 +4363,13 @@
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="J174" s="0" t="s">
         <v>16</v>
@@ -4262,13 +4377,13 @@
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="J175" s="0" t="s">
         <v>16</v>
@@ -4276,13 +4391,13 @@
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B176" s="0" t="s">
         <v>284</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="J176" s="0" t="s">
         <v>16</v>
@@ -4290,10 +4405,10 @@
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
@@ -4304,13 +4419,13 @@
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="J178" s="0" t="s">
         <v>16</v>
@@ -4318,13 +4433,13 @@
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J179" s="0" t="s">
         <v>16</v>
@@ -4332,13 +4447,13 @@
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J180" s="0" t="s">
         <v>16</v>
@@ -4346,13 +4461,13 @@
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J181" s="0" t="s">
         <v>16</v>
@@ -4360,13 +4475,13 @@
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J182" s="0" t="s">
         <v>16</v>
@@ -4374,13 +4489,13 @@
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J183" s="0" t="s">
         <v>16</v>
@@ -4388,13 +4503,13 @@
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J184" s="0" t="s">
         <v>16</v>
@@ -4402,13 +4517,13 @@
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="J185" s="0" t="s">
         <v>16</v>
@@ -4416,13 +4531,13 @@
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>256</v>
+        <v>13</v>
       </c>
       <c r="J186" s="0" t="s">
         <v>16</v>
@@ -4430,13 +4545,13 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>37</v>
+        <v>285</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J187" s="0" t="s">
         <v>16</v>
@@ -4446,8 +4561,8 @@
       <c r="A188" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>296</v>
+      <c r="B188" s="0" t="s">
+        <v>297</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>34</v>
@@ -4460,8 +4575,8 @@
       <c r="A189" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B189" s="0" t="s">
-        <v>297</v>
+      <c r="B189" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>34</v>
@@ -4475,7 +4590,7 @@
         <v>37</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>34</v>
@@ -4489,7 +4604,7 @@
         <v>37</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>34</v>
@@ -4503,13 +4618,10 @@
         <v>37</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F192" s="0" t="s">
-        <v>299</v>
+        <v>34</v>
       </c>
       <c r="J192" s="0" t="s">
         <v>16</v>
@@ -4520,13 +4632,13 @@
         <v>37</v>
       </c>
       <c r="B193" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D193" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F193" s="0" t="s">
         <v>301</v>
-      </c>
-      <c r="D193" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E193" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="J193" s="0" t="s">
         <v>16</v>
@@ -4537,10 +4649,13 @@
         <v>37</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>13</v>
+      </c>
+      <c r="E194" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="J194" s="0" t="s">
         <v>16</v>
@@ -4551,10 +4666,10 @@
         <v>37</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="J195" s="0" t="s">
         <v>16</v>
@@ -4565,16 +4680,10 @@
         <v>37</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E196" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G196" s="0" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J196" s="0" t="s">
         <v>16</v>
@@ -4585,10 +4694,16 @@
         <v>37</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="E197" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G197" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="J197" s="0" t="s">
         <v>16</v>
@@ -4599,7 +4714,7 @@
         <v>37</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>34</v>
@@ -4613,10 +4728,10 @@
         <v>37</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>256</v>
+        <v>34</v>
       </c>
       <c r="J199" s="0" t="s">
         <v>16</v>
@@ -4627,10 +4742,10 @@
         <v>37</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J200" s="0" t="s">
         <v>16</v>
@@ -4641,10 +4756,10 @@
         <v>37</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J201" s="0" t="s">
         <v>16</v>
@@ -4652,13 +4767,13 @@
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>310</v>
+        <v>37</v>
       </c>
       <c r="B202" s="0" t="s">
         <v>311</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J202" s="0" t="s">
         <v>16</v>
@@ -4666,10 +4781,10 @@
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>34</v>
@@ -4680,10 +4795,10 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>34</v>
@@ -4694,10 +4809,10 @@
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>34</v>
@@ -4708,10 +4823,10 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>34</v>
@@ -4722,10 +4837,10 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>34</v>
@@ -4736,19 +4851,13 @@
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>318</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E208" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G208" s="0" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="J208" s="0" t="s">
         <v>16</v>
@@ -4756,13 +4865,19 @@
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>37</v>
+        <v>319</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="E209" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G209" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="J209" s="0" t="s">
         <v>16</v>
@@ -4773,13 +4888,10 @@
         <v>37</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F210" s="0" t="s">
-        <v>319</v>
+        <v>34</v>
       </c>
       <c r="J210" s="0" t="s">
         <v>16</v>
@@ -4790,27 +4902,27 @@
         <v>37</v>
       </c>
       <c r="B211" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F211" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="D211" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E211" s="0" t="s">
-        <v>322</v>
-      </c>
       <c r="J211" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B212" s="0" t="s">
         <v>323</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E212" s="0" t="s">
         <v>324</v>
@@ -4827,9 +4939,9 @@
         <v>325</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G213" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E213" s="0" t="s">
         <v>326</v>
       </c>
       <c r="J213" s="0" t="s">
@@ -4847,13 +4959,10 @@
         <v>13</v>
       </c>
       <c r="G214" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="I214" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="J214" s="0" t="s">
-        <v>328</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4867,10 +4976,10 @@
         <v>13</v>
       </c>
       <c r="G215" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="I215" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="J215" s="0" t="s">
         <v>330</v>
@@ -4884,10 +4993,16 @@
         <v>331</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="G216" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="I216" s="0" t="s">
+        <v>327</v>
       </c>
       <c r="J216" s="0" t="s">
-        <v>16</v>
+        <v>332</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4895,13 +5010,10 @@
         <v>10</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E217" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J217" s="0" t="s">
         <v>16</v>
@@ -4912,7 +5024,7 @@
         <v>10</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D218" s="0" t="s">
         <v>13</v>
@@ -4920,11 +5032,8 @@
       <c r="E218" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I218" s="0" t="s">
-        <v>332</v>
-      </c>
       <c r="J218" s="0" t="s">
-        <v>334</v>
+        <v>16</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,7 +5050,7 @@
         <v>14</v>
       </c>
       <c r="I219" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="J219" s="0" t="s">
         <v>336</v>
@@ -4952,7 +5061,7 @@
         <v>10</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>96</v>
+        <v>337</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>13</v>
@@ -4961,10 +5070,10 @@
         <v>14</v>
       </c>
       <c r="I220" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4972,7 +5081,7 @@
         <v>10</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>338</v>
+        <v>98</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>13</v>
@@ -4981,7 +5090,7 @@
         <v>14</v>
       </c>
       <c r="I221" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="J221" s="0" t="s">
         <v>339</v>
@@ -4995,10 +5104,16 @@
         <v>340</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>60</v>
+        <v>13</v>
+      </c>
+      <c r="E222" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I222" s="0" t="s">
+        <v>334</v>
       </c>
       <c r="J222" s="0" t="s">
-        <v>16</v>
+        <v>341</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5006,10 +5121,10 @@
         <v>10</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J223" s="0" t="s">
         <v>16</v>
@@ -5020,10 +5135,10 @@
         <v>10</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="J224" s="0" t="s">
         <v>16</v>
@@ -5034,7 +5149,7 @@
         <v>10</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>34</v>
@@ -5045,10 +5160,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>34</v>
@@ -5059,10 +5174,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>34</v>
@@ -5071,7 +5186,22 @@
         <v>16</v>
       </c>
     </row>
+    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J228" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J228"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5079,5 +5209,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding data collection from twitter usding the filter api
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -1199,7 +1199,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J228"/>
@@ -1207,7 +1207,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+      <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1254,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>37</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>37</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>37</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>37</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>37</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>37</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>37</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>37</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>10</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>37</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>37</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>37</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>10</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>10</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>10</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>72</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>72</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>72</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>72</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>81</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>85</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>81</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>81</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>81</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>81</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>81</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>81</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>81</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>81</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>81</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>81</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>81</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>106</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>108</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>81</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>81</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>81</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>81</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>81</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>81</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>81</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>81</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>81</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>81</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>81</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>81</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>81</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>81</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>81</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>81</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>106</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>108</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>81</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>81</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>81</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>81</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>148</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>148</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>148</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>148</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>148</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>158</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>148</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>148</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>148</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>148</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>148</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>166</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>166</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>166</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>166</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>166</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>166</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>166</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>166</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>166</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>166</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>166</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>166</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>166</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>166</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>166</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>166</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>166</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>166</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>166</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>166</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>204</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>166</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>166</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>166</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>166</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>166</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>166</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>166</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>166</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>215</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>215</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>215</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>215</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>215</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>215</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>215</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>215</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>215</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>215</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>215</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>215</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>215</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>215</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>215</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>215</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>215</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>215</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>215</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>215</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>215</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>248</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>248</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>248</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>248</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>248</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>248</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>248</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>248</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>259</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>259</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>259</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>259</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>259</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>265</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>265</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>265</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>265</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>265</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>271</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>271</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>271</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>271</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>271</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>271</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>271</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>271</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>280</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>280</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>280</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>280</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>285</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>285</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>285</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>285</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>37</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>37</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>37</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>37</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>37</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>37</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>37</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>37</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>37</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>37</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>37</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>37</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>37</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>37</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>37</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>312</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>312</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
         <v>312</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
         <v>312</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
         <v>312</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
         <v>312</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
         <v>319</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>37</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>37</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
         <v>37</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
         <v>10</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
         <v>10</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
         <v>10</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>10</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>10</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>10</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>10</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>10</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>10</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
         <v>10</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>10</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
         <v>81</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
         <v>81</v>
       </c>
@@ -5201,7 +5201,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J228"/>
+  <autoFilter ref="A1:J228">
+    <filterColumn colId="3">
+      <customFilters and="true">
+        <customFilter operator="equal" val="indicator"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
1. tweet collection done 2. NUIG algorithms integration done
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$228</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$236</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$J$229</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="352">
   <si>
     <t xml:space="preserve">data_family</t>
   </si>
@@ -70,7 +71,7 @@
     <t xml:space="preserve">people</t>
   </si>
   <si>
-    <t xml:space="preserve">reporting_period, case_status</t>
+    <t xml:space="preserve">source, reporting_period, case_status</t>
   </si>
   <si>
     <t xml:space="preserve">[]</t>
@@ -196,6 +197,12 @@
     <t xml:space="preserve">[{'variable': 'period_type', 'value': 'date'}]</t>
   </si>
   <si>
+    <t xml:space="preserve">reporting_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{'variable': 'period_type', 'value': 'instant'}]</t>
+  </si>
+  <si>
     <t xml:space="preserve">reporting_week</t>
   </si>
   <si>
@@ -280,9 +287,6 @@
     <t xml:space="preserve">people/people</t>
   </si>
   <si>
-    <t xml:space="preserve">03_patients</t>
-  </si>
-  <si>
     <t xml:space="preserve">severity</t>
   </si>
   <si>
@@ -343,15 +347,9 @@
     <t xml:space="preserve">[{'variable': 'bed_type', 'value': 'icu'}]</t>
   </si>
   <si>
-    <t xml:space="preserve">04_patient</t>
-  </si>
-  <si>
     <t xml:space="preserve">care_type</t>
   </si>
   <si>
-    <t xml:space="preserve">05_patient</t>
-  </si>
-  <si>
     <t xml:space="preserve">bed_type</t>
   </si>
   <si>
@@ -469,7 +467,7 @@
     <t xml:space="preserve">beds_occupancy</t>
   </si>
   <si>
-    <t xml:space="preserve">04tests</t>
+    <t xml:space="preserve">04_tests</t>
   </si>
   <si>
     <t xml:space="preserve">performed_tests</t>
@@ -499,9 +497,6 @@
     <t xml:space="preserve">[{'variable': 'test_result', 'value': 'unknown'}]</t>
   </si>
   <si>
-    <t xml:space="preserve">05tests</t>
-  </si>
-  <si>
     <t xml:space="preserve">available_tests</t>
   </si>
   <si>
@@ -635,9 +630,6 @@
   </si>
   <si>
     <t xml:space="preserve">vaccination_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06_vaccination</t>
   </si>
   <si>
     <t xml:space="preserve">population_type</t>
@@ -983,9 +975,6 @@
     <t xml:space="preserve">gdpr_compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">14_variants</t>
-  </si>
-  <si>
     <t xml:space="preserve">number_detections_variant</t>
   </si>
   <si>
@@ -1068,6 +1057,30 @@
   </si>
   <si>
     <t xml:space="preserve">comorbidity_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_created_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source, reporting_period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">article_alert</t>
   </si>
 </sst>
 </file>
@@ -1077,13 +1090,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1102,13 +1114,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1173,7 +1178,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1202,15 +1207,15 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J228"/>
+  <dimension ref="A1:J236"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="B235" activeCellId="0" sqref="B235"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.7"/>
@@ -1222,7 +1227,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.12"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -1277,7 +1282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -1303,7 +1308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1329,7 +1334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
@@ -1355,7 +1360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
@@ -1407,7 +1412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
@@ -1433,7 +1438,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1464,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
@@ -1485,7 +1490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>10</v>
       </c>
@@ -1656,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>37</v>
       </c>
@@ -1670,7 +1675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
@@ -1684,7 +1689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
@@ -1698,7 +1703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1720,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>10</v>
       </c>
@@ -1729,7 +1734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>37</v>
       </c>
@@ -1746,7 +1751,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>37</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +1791,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>37</v>
       </c>
@@ -1796,41 +1801,44 @@
       <c r="D28" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="E28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="H30" s="0" t="s">
         <v>65</v>
       </c>
       <c r="J30" s="0" t="s">
@@ -1845,10 +1853,10 @@
         <v>66</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>16</v>
@@ -1859,13 +1867,13 @@
         <v>10</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="E32" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>16</v>
@@ -1876,13 +1884,13 @@
         <v>10</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>16</v>
@@ -1890,19 +1898,16 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="D34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>16</v>
@@ -1910,10 +1915,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>13</v>
@@ -1924,19 +1929,16 @@
       <c r="G35" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="I35" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="J35" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>13</v>
@@ -1948,15 +1950,15 @@
         <v>53</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>77</v>
@@ -1971,7 +1973,7 @@
         <v>53</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J37" s="0" t="s">
         <v>78</v>
@@ -1979,7 +1981,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>79</v>
@@ -1994,7 +1996,7 @@
         <v>53</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J38" s="0" t="s">
         <v>80</v>
@@ -2002,30 +2004,36 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="D39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="J39" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="0" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="J40" s="0" t="s">
         <v>16</v>
@@ -2033,13 +2041,16 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="D41" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="J41" s="0" t="s">
         <v>16</v>
@@ -2047,16 +2058,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>87</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J42" s="0" t="s">
         <v>16</v>
@@ -2064,7 +2072,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>88</v>
@@ -2075,19 +2083,16 @@
       <c r="E43" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="J43" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>13</v>
@@ -2096,18 +2101,15 @@
         <v>14</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>91</v>
@@ -2119,10 +2121,10 @@
         <v>14</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I45" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="J45" s="0" t="s">
         <v>78</v>
@@ -2130,7 +2132,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>92</v>
@@ -2142,21 +2144,21 @@
         <v>14</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I46" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I46" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J46" s="0" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>13</v>
@@ -2165,21 +2167,21 @@
         <v>14</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I47" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I47" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J47" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
@@ -2188,21 +2190,21 @@
         <v>14</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I48" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I48" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J48" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
@@ -2211,21 +2213,21 @@
         <v>14</v>
       </c>
       <c r="G49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I49" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I49" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J49" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
@@ -2234,21 +2236,21 @@
         <v>14</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I50" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I50" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J50" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
@@ -2257,21 +2259,21 @@
         <v>14</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I51" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J51" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>13</v>
@@ -2280,35 +2282,44 @@
         <v>14</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I52" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I52" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="J52" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J53" s="0" t="s">
         <v>106</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>45</v>
@@ -2319,13 +2330,13 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J55" s="0" t="s">
         <v>16</v>
@@ -2333,121 +2344,115 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D58" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>116</v>
+        <v>63</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I60" s="0" t="s">
         <v>115</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J62" s="0" t="s">
         <v>16</v>
@@ -2455,19 +2460,19 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J63" s="0" t="s">
         <v>16</v>
@@ -2475,254 +2480,260 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D64" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G64" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I64" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D65" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G65" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I65" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I65" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J65" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D66" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G66" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I66" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I66" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J66" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D67" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E67" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G67" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I67" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I67" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J67" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D68" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E68" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G68" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I68" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I68" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J68" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D69" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E69" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G69" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I69" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I69" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J69" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D70" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G70" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I70" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I70" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J70" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D71" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E71" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G71" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I71" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I71" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J71" s="0" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D72" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E72" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G72" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I72" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I72" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J72" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D73" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E73" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E73" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="G73" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I73" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="I73" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="J73" s="0" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>45</v>
+        <v>69</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>120</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>45</v>
@@ -2733,10 +2744,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>45</v>
@@ -2747,16 +2758,13 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E77" s="0" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J77" s="0" t="s">
         <v>16</v>
@@ -2764,16 +2772,16 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D78" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="E78" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="J78" s="0" t="s">
         <v>16</v>
@@ -2781,16 +2789,16 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D79" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E79" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="E79" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="J79" s="0" t="s">
         <v>16</v>
@@ -2798,19 +2806,16 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="J80" s="0" t="s">
         <v>16</v>
@@ -2818,122 +2823,128 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B81" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B81" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="D81" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I81" s="0" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>151</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I82" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I82" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="J82" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I83" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E83" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="J83" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I84" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I84" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="J84" s="0" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>148</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>16</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="J86" s="0" t="s">
         <v>16</v>
@@ -2941,33 +2952,30 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="J87" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="J88" s="0" t="s">
         <v>16</v>
@@ -2975,16 +2983,16 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="J89" s="0" t="s">
         <v>16</v>
@@ -2992,16 +3000,16 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="J90" s="0" t="s">
         <v>16</v>
@@ -3009,16 +3017,16 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D91" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E91" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="E91" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="J91" s="0" t="s">
         <v>16</v>
@@ -3026,19 +3034,16 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="G92" s="0" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="J92" s="0" t="s">
         <v>16</v>
@@ -3046,19 +3051,19 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="J93" s="0" t="s">
         <v>16</v>
@@ -3066,10 +3071,10 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>169</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>13</v>
@@ -3078,21 +3083,18 @@
         <v>14</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="I94" s="0" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>170</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>13</v>
@@ -3101,21 +3103,21 @@
         <v>14</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I95" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="J95" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="J95" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>13</v>
@@ -3124,21 +3126,21 @@
         <v>14</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>13</v>
@@ -3147,21 +3149,21 @@
         <v>14</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>13</v>
@@ -3170,21 +3172,21 @@
         <v>14</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>13</v>
@@ -3193,21 +3195,21 @@
         <v>14</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>13</v>
@@ -3216,21 +3218,21 @@
         <v>14</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I100" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>13</v>
@@ -3239,21 +3241,21 @@
         <v>14</v>
       </c>
       <c r="G101" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I101" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>13</v>
@@ -3262,21 +3264,21 @@
         <v>14</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I102" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>13</v>
@@ -3285,21 +3287,21 @@
         <v>14</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>13</v>
@@ -3308,21 +3310,21 @@
         <v>14</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>13</v>
@@ -3331,21 +3333,21 @@
         <v>14</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I105" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>13</v>
@@ -3354,21 +3356,21 @@
         <v>14</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I106" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>13</v>
@@ -3377,21 +3379,21 @@
         <v>14</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I107" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D108" s="0" t="s">
         <v>13</v>
@@ -3400,21 +3402,21 @@
         <v>14</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I108" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D109" s="0" t="s">
         <v>13</v>
@@ -3423,21 +3425,21 @@
         <v>14</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I109" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>13</v>
@@ -3446,35 +3448,44 @@
         <v>14</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I110" s="0" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="I111" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="J111" s="0" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>204</v>
+        <v>164</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D112" s="0" t="s">
         <v>45</v>
@@ -3485,10 +3496,10 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>45</v>
@@ -3499,13 +3510,13 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J114" s="0" t="s">
         <v>16</v>
@@ -3513,13 +3524,13 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J115" s="0" t="s">
         <v>16</v>
@@ -3527,10 +3538,10 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>45</v>
@@ -3541,10 +3552,10 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D117" s="0" t="s">
         <v>45</v>
@@ -3555,10 +3566,10 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>45</v>
@@ -3569,10 +3580,10 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>45</v>
@@ -3581,15 +3592,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J120" s="0" t="s">
         <v>16</v>
@@ -3597,13 +3608,13 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J121" s="0" t="s">
         <v>16</v>
@@ -3611,13 +3622,13 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J122" s="0" t="s">
         <v>16</v>
@@ -3625,10 +3636,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>13</v>
@@ -3639,160 +3650,160 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I124" s="0" t="s">
-        <v>217</v>
-      </c>
       <c r="J124" s="0" t="s">
-        <v>219</v>
+        <v>16</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B125" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B125" s="0" t="s">
-        <v>220</v>
-      </c>
       <c r="D125" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I125" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I126" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I129" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I131" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J131" s="0" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="I132" s="0" t="s">
+        <v>214</v>
       </c>
       <c r="J132" s="0" t="s">
-        <v>16</v>
+        <v>230</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>45</v>
@@ -3803,10 +3814,10 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>45</v>
@@ -3817,10 +3828,10 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>45</v>
@@ -3831,41 +3842,41 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D136" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J136" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D137" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J136" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B137" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="D137" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="J137" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J138" s="0" t="s">
         <v>16</v>
@@ -3873,13 +3884,13 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="J139" s="0" t="s">
         <v>16</v>
@@ -3887,13 +3898,13 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J140" s="0" t="s">
         <v>16</v>
@@ -3901,13 +3912,13 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J141" s="0" t="s">
         <v>16</v>
@@ -3915,13 +3926,13 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D142" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J142" s="0" t="s">
         <v>16</v>
@@ -3929,27 +3940,27 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D143" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J143" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="D144" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="J143" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B144" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="D144" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="J144" s="0" t="s">
         <v>16</v>
@@ -3957,13 +3968,13 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J145" s="0" t="s">
         <v>16</v>
@@ -3971,13 +3982,13 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J146" s="0" t="s">
         <v>16</v>
@@ -3985,10 +3996,10 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D147" s="0" t="s">
         <v>13</v>
@@ -3997,15 +4008,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="J148" s="0" t="s">
         <v>16</v>
@@ -4013,13 +4024,13 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B149" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="B149" s="0" t="s">
-        <v>252</v>
-      </c>
       <c r="D149" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="J149" s="0" t="s">
         <v>16</v>
@@ -4027,13 +4038,13 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="J150" s="0" t="s">
         <v>16</v>
@@ -4041,13 +4052,13 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J151" s="0" t="s">
         <v>16</v>
@@ -4055,10 +4066,10 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>45</v>
@@ -4069,10 +4080,10 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>45</v>
@@ -4083,13 +4094,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="J154" s="0" t="s">
         <v>16</v>
@@ -4097,13 +4108,13 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="J155" s="0" t="s">
         <v>16</v>
@@ -4111,10 +4122,10 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D156" s="0" t="s">
         <v>13</v>
@@ -4125,13 +4136,13 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J157" s="0" t="s">
         <v>16</v>
@@ -4139,13 +4150,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B158" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B158" s="0" t="s">
-        <v>263</v>
-      </c>
       <c r="D158" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J158" s="0" t="s">
         <v>16</v>
@@ -4153,13 +4164,13 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J159" s="0" t="s">
         <v>16</v>
@@ -4167,13 +4178,13 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="J160" s="0" t="s">
         <v>16</v>
@@ -4181,10 +4192,10 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>13</v>
@@ -4195,13 +4206,13 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D162" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J162" s="0" t="s">
         <v>16</v>
@@ -4209,13 +4220,13 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B163" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="B163" s="0" t="s">
-        <v>269</v>
-      </c>
       <c r="D163" s="0" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="J163" s="0" t="s">
         <v>16</v>
@@ -4223,13 +4234,13 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J164" s="0" t="s">
         <v>16</v>
@@ -4237,13 +4248,13 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="J165" s="0" t="s">
         <v>16</v>
@@ -4251,10 +4262,10 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>13</v>
@@ -4265,10 +4276,10 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D167" s="0" t="s">
         <v>13</v>
@@ -4279,13 +4290,13 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B168" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B168" s="0" t="s">
-        <v>275</v>
-      </c>
       <c r="D168" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>16</v>
@@ -4293,13 +4304,13 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="J169" s="0" t="s">
         <v>16</v>
@@ -4307,13 +4318,13 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J170" s="0" t="s">
         <v>16</v>
@@ -4321,262 +4332,262 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B171" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J171" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J172" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J173" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B174" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="D171" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J171" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B172" s="0" t="s">
+      <c r="D174" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J174" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B175" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="D172" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="J172" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
+      <c r="D175" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J175" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B176" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B173" s="0" t="s">
+      <c r="D176" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J176" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B177" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="D173" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J173" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B174" s="0" t="s">
+      <c r="D177" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J177" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
         <v>282</v>
       </c>
-      <c r="D174" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J174" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B175" s="0" t="s">
+      <c r="B178" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="D175" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J175" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B176" s="0" t="s">
+      <c r="D178" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J178" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B179" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="D176" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="J176" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
+      <c r="D179" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J179" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B180" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B177" s="0" t="s">
+      <c r="D180" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J180" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B181" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="D177" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J177" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B178" s="0" t="s">
+      <c r="D181" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J181" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B182" s="0" t="s">
         <v>287</v>
       </c>
-      <c r="D178" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J178" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B179" s="0" t="s">
+      <c r="D182" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J182" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B183" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="D179" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J179" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B180" s="0" t="s">
+      <c r="D183" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J183" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B184" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="D180" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J180" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B181" s="0" t="s">
+      <c r="D184" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J184" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B185" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="D181" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J181" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B182" s="0" t="s">
+      <c r="D185" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J185" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B186" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="D182" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J182" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B183" s="0" t="s">
+      <c r="D186" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J186" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B187" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="D183" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J183" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B184" s="0" t="s">
+      <c r="D187" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J187" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B188" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="D184" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J184" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B185" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="D185" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="J185" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B186" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="D186" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J186" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B187" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="D187" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="J187" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B188" s="0" t="s">
-        <v>297</v>
-      </c>
       <c r="D188" s="0" t="s">
-        <v>34</v>
+        <v>255</v>
       </c>
       <c r="J188" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B189" s="3" t="s">
-        <v>298</v>
+      <c r="B189" s="0" t="s">
+        <v>294</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>34</v>
@@ -4585,12 +4596,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B190" s="0" t="s">
-        <v>299</v>
+      <c r="B190" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>34</v>
@@ -4599,12 +4610,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>34</v>
@@ -4613,12 +4624,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D192" s="0" t="s">
         <v>34</v>
@@ -4627,108 +4638,108 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F193" s="0" t="s">
-        <v>301</v>
+        <v>34</v>
       </c>
       <c r="J193" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E194" s="0" t="s">
-        <v>54</v>
+        <v>36</v>
+      </c>
+      <c r="F194" s="0" t="s">
+        <v>298</v>
       </c>
       <c r="J194" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="E195" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="J195" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="J196" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E197" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G197" s="0" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="J197" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
+      </c>
+      <c r="E198" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G198" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="J198" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>34</v>
@@ -4737,68 +4748,68 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>258</v>
+        <v>34</v>
       </c>
       <c r="J200" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J201" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J202" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>312</v>
+        <v>37</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>34</v>
+        <v>255</v>
       </c>
       <c r="J203" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>34</v>
@@ -4807,12 +4818,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>34</v>
@@ -4821,12 +4832,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B206" s="0" t="s">
         <v>312</v>
-      </c>
-      <c r="B206" s="0" t="s">
-        <v>316</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>34</v>
@@ -4835,12 +4846,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>34</v>
@@ -4849,12 +4860,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>34</v>
@@ -4863,52 +4874,49 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E209" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J209" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E210" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="G209" s="0" t="s">
+      <c r="G210" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="J209" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B210" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="D210" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="J210" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F211" s="0" t="s">
-        <v>321</v>
+        <v>34</v>
       </c>
       <c r="J211" s="0" t="s">
         <v>16</v>
@@ -4919,129 +4927,129 @@
         <v>37</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D212" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="J212" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D213" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E212" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="J212" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B213" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="D213" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="E213" s="0" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="J213" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G214" s="0" t="s">
-        <v>328</v>
+        <v>63</v>
+      </c>
+      <c r="E214" s="0" t="s">
+        <v>322</v>
       </c>
       <c r="J214" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G215" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="I215" s="0" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J215" s="0" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D216" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G216" s="0" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I216" s="0" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="J216" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>45</v>
+        <v>13</v>
+      </c>
+      <c r="G217" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="I217" s="0" t="s">
+        <v>323</v>
       </c>
       <c r="J217" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E218" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="J218" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>13</v>
@@ -5049,19 +5057,16 @@
       <c r="E219" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I219" s="0" t="s">
-        <v>334</v>
-      </c>
       <c r="J219" s="0" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>13</v>
@@ -5070,18 +5075,18 @@
         <v>14</v>
       </c>
       <c r="I220" s="0" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>98</v>
+        <v>333</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>13</v>
@@ -5090,18 +5095,18 @@
         <v>14</v>
       </c>
       <c r="I221" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="J221" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="J221" s="0" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="222" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>340</v>
+        <v>99</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>13</v>
@@ -5110,60 +5115,66 @@
         <v>14</v>
       </c>
       <c r="I222" s="0" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="J222" s="0" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>61</v>
+        <v>13</v>
+      </c>
+      <c r="E223" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I223" s="0" t="s">
+        <v>330</v>
       </c>
       <c r="J223" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J224" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="J225" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>34</v>
@@ -5172,12 +5183,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>34</v>
@@ -5186,12 +5197,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>34</v>
@@ -5200,11 +5211,129 @@
         <v>16</v>
       </c>
     </row>
+    <row r="229" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="D229" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J229" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="D230" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="J230" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="D231" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J231" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D232" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J232" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="D233" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J233" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B234" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D234" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J234" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="D235" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G235" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="J235" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="D236" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G236" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="J236" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J228">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:J236">
+    <filterColumn colId="0">
       <customFilters and="true">
-        <customFilter operator="equal" val="indicator"/>
+        <customFilter operator="equal" val="12_population_study"/>
       </customFilters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
compute indicators from published data
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -1083,7 +1083,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1106,7 +1105,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1191,10 +1189,10 @@
   <dimension ref="A1:J228"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.21"/>
@@ -1202,13 +1200,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="11" style="0" width="8.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -1289,7 +1288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
@@ -1341,7 +1340,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +1418,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>10</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>10</v>
       </c>
@@ -1502,7 +1501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>37</v>
       </c>
@@ -1516,7 +1515,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>37</v>
       </c>
@@ -1533,7 +1532,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>37</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>37</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>37</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>37</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>10</v>
       </c>
@@ -1677,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>37</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>37</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>37</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>37</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>10</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>10</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>10</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>10</v>
       </c>
@@ -1839,7 +1838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>73</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>73</v>
       </c>
@@ -1882,7 +1881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>73</v>
       </c>
@@ -1905,7 +1904,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>73</v>
       </c>
@@ -1928,7 +1927,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>73</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>82</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>73</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>86</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>82</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>82</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>82</v>
       </c>
@@ -2050,7 +2049,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>82</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>82</v>
       </c>
@@ -2090,7 +2089,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>82</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>82</v>
       </c>
@@ -2130,7 +2129,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>82</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>82</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>82</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>82</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>106</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>108</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>82</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>82</v>
       </c>
@@ -2269,7 +2268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>82</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>82</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>82</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>82</v>
       </c>
@@ -2337,7 +2336,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>82</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>82</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>82</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>82</v>
       </c>
@@ -2408,7 +2407,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>82</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>82</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>82</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>82</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>82</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>82</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>82</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>82</v>
       </c>
@@ -2568,7 +2567,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>82</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>106</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>108</v>
       </c>
@@ -2616,7 +2615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>82</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>82</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>82</v>
       </c>
@@ -2664,7 +2663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>82</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>147</v>
       </c>
@@ -2701,7 +2700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>147</v>
       </c>
@@ -2724,7 +2723,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>147</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>147</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>147</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>158</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>147</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>147</v>
       </c>
@@ -2841,7 +2840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>147</v>
       </c>
@@ -2858,7 +2857,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>147</v>
       </c>
@@ -2875,7 +2874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>147</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>147</v>
       </c>
@@ -2909,7 +2908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>166</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>166</v>
       </c>
@@ -2949,7 +2948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>166</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>166</v>
       </c>
@@ -3064,7 +3063,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>166</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>166</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>166</v>
       </c>
@@ -3133,7 +3132,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>166</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>166</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>166</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>166</v>
       </c>
@@ -3225,7 +3224,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>166</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>166</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>166</v>
       </c>
@@ -3294,7 +3293,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>166</v>
       </c>
@@ -3317,7 +3316,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>166</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>166</v>
       </c>
@@ -3354,7 +3353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>204</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>166</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>166</v>
       </c>
@@ -3396,7 +3395,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>166</v>
       </c>
@@ -3410,7 +3409,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>166</v>
       </c>
@@ -3424,7 +3423,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>166</v>
       </c>
@@ -3438,7 +3437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>166</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>166</v>
       </c>
@@ -3466,7 +3465,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>166</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>166</v>
       </c>
@@ -3494,7 +3493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>215</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>215</v>
       </c>
@@ -3522,7 +3521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>215</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>215</v>
       </c>
@@ -3556,7 +3555,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>215</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>215</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>215</v>
       </c>
@@ -3607,7 +3606,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>215</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>215</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>215</v>
       </c>
@@ -3658,7 +3657,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>215</v>
       </c>
@@ -3672,7 +3671,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>215</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>215</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>215</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>215</v>
       </c>
@@ -3728,7 +3727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>215</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>215</v>
       </c>
@@ -3756,7 +3755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>215</v>
       </c>
@@ -3770,7 +3769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>215</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>215</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>215</v>
       </c>
@@ -3812,7 +3811,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>215</v>
       </c>
@@ -3826,7 +3825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>215</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>215</v>
       </c>
@@ -3854,7 +3853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>248</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>248</v>
       </c>
@@ -3882,7 +3881,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>248</v>
       </c>
@@ -3896,7 +3895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>248</v>
       </c>
@@ -3910,7 +3909,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>248</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>248</v>
       </c>
@@ -3938,7 +3937,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>248</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>248</v>
       </c>
@@ -3966,7 +3965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>248</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>259</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>259</v>
       </c>
@@ -4008,7 +4007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>259</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>259</v>
       </c>
@@ -4036,7 +4035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>259</v>
       </c>
@@ -4050,7 +4049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>265</v>
       </c>
@@ -4064,7 +4063,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>265</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>265</v>
       </c>
@@ -4092,7 +4091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>265</v>
       </c>
@@ -4106,7 +4105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>265</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>271</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>271</v>
       </c>
@@ -4148,7 +4147,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>271</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>271</v>
       </c>
@@ -4176,7 +4175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>271</v>
       </c>
@@ -4190,7 +4189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>271</v>
       </c>
@@ -4204,7 +4203,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>271</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>271</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>280</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>280</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>280</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>280</v>
       </c>
@@ -4288,7 +4287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>285</v>
       </c>
@@ -4302,7 +4301,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>285</v>
       </c>
@@ -4316,7 +4315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>285</v>
       </c>
@@ -4330,7 +4329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>285</v>
       </c>
@@ -4344,7 +4343,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>285</v>
       </c>
@@ -4358,7 +4357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>285</v>
       </c>
@@ -4372,7 +4371,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>285</v>
       </c>
@@ -4386,7 +4385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
         <v>285</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>285</v>
       </c>
@@ -4414,7 +4413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>285</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>285</v>
       </c>
@@ -4442,7 +4441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>37</v>
       </c>
@@ -4456,7 +4455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>37</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>37</v>
       </c>
@@ -4484,7 +4483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>37</v>
       </c>
@@ -4498,7 +4497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>37</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>37</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>37</v>
       </c>
@@ -4546,7 +4545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>37</v>
       </c>
@@ -4560,7 +4559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>37</v>
       </c>
@@ -4574,7 +4573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>37</v>
       </c>
@@ -4594,7 +4593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>37</v>
       </c>
@@ -4608,7 +4607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>37</v>
       </c>
@@ -4622,7 +4621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>37</v>
       </c>
@@ -4636,7 +4635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>37</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>37</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>312</v>
       </c>
@@ -4678,7 +4677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>312</v>
       </c>
@@ -4692,7 +4691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>312</v>
       </c>
@@ -4706,7 +4705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
         <v>312</v>
       </c>
@@ -4720,7 +4719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
         <v>312</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
         <v>312</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
         <v>319</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
         <v>37</v>
       </c>
@@ -4782,7 +4781,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>37</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>37</v>
       </c>
@@ -4816,7 +4815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
         <v>10</v>
       </c>
@@ -4833,7 +4832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
         <v>10</v>
       </c>
@@ -4850,7 +4849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
         <v>10</v>
       </c>
@@ -4870,7 +4869,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
         <v>10</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
         <v>10</v>
       </c>
@@ -4904,7 +4903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>10</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>10</v>
       </c>
@@ -4941,7 +4940,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>10</v>
       </c>
@@ -4961,7 +4960,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>10</v>
       </c>
@@ -5015,7 +5014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
         <v>10</v>
       </c>
@@ -5029,7 +5028,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
         <v>10</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
         <v>10</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>10</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
         <v>82</v>
       </c>
@@ -5085,7 +5084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Fixing aggregation and private fields processing
</commit_message>
<xml_diff>
--- a/pandem2source/data/list-of-variables.xlsx
+++ b/pandem2source/data/list-of-variables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="359">
   <si>
     <t xml:space="preserve">data_family</t>
   </si>
@@ -1231,9 +1231,9 @@
   <dimension ref="A1:J239"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="E235" activeCellId="0" sqref="E235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5329,6 +5329,9 @@
       <c r="D235" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="E235" s="0" t="s">
+        <v>69</v>
+      </c>
       <c r="G235" s="0" t="s">
         <v>354</v>
       </c>

</xml_diff>